<commit_message>
Fix minor bugs in configuration writer
</commit_message>
<xml_diff>
--- a/PRO1/step_3/results/res_bus/vm_pu.xlsx
+++ b/PRO1/step_3/results/res_bus/vm_pu.xlsx
@@ -442,61 +442,61 @@
         <v>1.03</v>
       </c>
       <c r="C2">
-        <v>1.022287785606226</v>
+        <v>1.022260583353094</v>
       </c>
       <c r="D2">
-        <v>1.017212861301559</v>
+        <v>1.016940257313771</v>
       </c>
       <c r="E2">
-        <v>1.008764243556</v>
+        <v>1.008114490211418</v>
       </c>
       <c r="F2">
-        <v>1.008320882087645</v>
+        <v>1.007655668441395</v>
       </c>
       <c r="G2">
-        <v>1.008018130962079</v>
+        <v>1.007338824045227</v>
       </c>
       <c r="H2">
-        <v>1.007668345802915</v>
+        <v>1.006988730819892</v>
       </c>
       <c r="I2">
-        <v>1.007425470330303</v>
+        <v>1.006720771515332</v>
       </c>
       <c r="J2">
-        <v>1.007462419686843</v>
+        <v>1.006757813590917</v>
       </c>
       <c r="K2">
-        <v>1.007221551487641</v>
+        <v>1.006514113243308</v>
       </c>
       <c r="L2">
-        <v>1.006920690104309</v>
+        <v>1.006206657536685</v>
       </c>
       <c r="M2">
-        <v>1.006875393711417</v>
+        <v>1.006158604565843</v>
       </c>
       <c r="N2">
-        <v>1.022734980948664</v>
+        <v>1.022730909631061</v>
       </c>
       <c r="O2">
-        <v>1.021430049851221</v>
+        <v>1.021304697376185</v>
       </c>
       <c r="P2">
-        <v>1.02067649724301</v>
+        <v>1.020551049093512</v>
       </c>
       <c r="Q2">
-        <v>1.007446506244054</v>
+        <v>1.006236606406304</v>
       </c>
       <c r="R2">
-        <v>1.021413915781757</v>
+        <v>1.020915632460395</v>
       </c>
       <c r="S2">
-        <v>1.008002208741513</v>
+        <v>1.006944760077447</v>
       </c>
       <c r="T2">
-        <v>1.006859489541038</v>
+        <v>1.006016915786869</v>
       </c>
       <c r="U2">
-        <v>1.008748309550161</v>
+        <v>1.007847062618489</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -507,61 +507,61 @@
         <v>1.03</v>
       </c>
       <c r="C3">
-        <v>1.022654000256572</v>
+        <v>1.022638495376116</v>
       </c>
       <c r="D3">
-        <v>1.017826244806614</v>
+        <v>1.01766432488076</v>
       </c>
       <c r="E3">
-        <v>1.009760920452753</v>
+        <v>1.009373809410904</v>
       </c>
       <c r="F3">
-        <v>1.009336673118919</v>
+        <v>1.0089393120861</v>
       </c>
       <c r="G3">
-        <v>1.009047031252258</v>
+        <v>1.008640318824184</v>
       </c>
       <c r="H3">
-        <v>1.008712747020375</v>
+        <v>1.008305856600393</v>
       </c>
       <c r="I3">
-        <v>1.008482582963286</v>
+        <v>1.008073363565869</v>
       </c>
       <c r="J3">
-        <v>1.008516235247874</v>
+        <v>1.00810706832818</v>
       </c>
       <c r="K3">
-        <v>1.008285332870445</v>
+        <v>1.007876057066866</v>
       </c>
       <c r="L3">
-        <v>1.007997198739165</v>
+        <v>1.007587781284021</v>
       </c>
       <c r="M3">
-        <v>1.007953904000022</v>
+        <v>1.007544463488786</v>
       </c>
       <c r="N3">
-        <v>1.023023459945867</v>
+        <v>1.023020853147901</v>
       </c>
       <c r="O3">
-        <v>1.021768915316444</v>
+        <v>1.021685534215698</v>
       </c>
       <c r="P3">
-        <v>1.021044215156406</v>
+        <v>1.020960772800367</v>
       </c>
       <c r="Q3">
-        <v>1.008500305159468</v>
+        <v>1.007839639001107</v>
       </c>
       <c r="R3">
-        <v>1.021752775894406</v>
+        <v>1.02142125391089</v>
       </c>
       <c r="S3">
-        <v>1.009031092779627</v>
+        <v>1.00837301488063</v>
       </c>
       <c r="T3">
-        <v>1.007937982793957</v>
+        <v>1.007528548753169</v>
       </c>
       <c r="U3">
-        <v>1.009744970703834</v>
+        <v>1.009106677710127</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -572,61 +572,61 @@
         <v>1.03</v>
       </c>
       <c r="C4">
-        <v>1.023030459902508</v>
+        <v>1.023012795258614</v>
       </c>
       <c r="D4">
-        <v>1.018457524838795</v>
+        <v>1.018269289579723</v>
       </c>
       <c r="E4">
-        <v>1.010787487972367</v>
+        <v>1.01033675842365</v>
       </c>
       <c r="F4">
-        <v>1.010382957995344</v>
+        <v>1.009926986977047</v>
       </c>
       <c r="G4">
-        <v>1.010106839194546</v>
+        <v>1.009646114445061</v>
       </c>
       <c r="H4">
-        <v>1.009788545020354</v>
+        <v>1.009327626104075</v>
       </c>
       <c r="I4">
-        <v>1.009571488756242</v>
+        <v>1.00907712174525</v>
       </c>
       <c r="J4">
-        <v>1.00960174003783</v>
+        <v>1.009107434743069</v>
       </c>
       <c r="K4">
-        <v>1.009381117377024</v>
+        <v>1.008881418796281</v>
       </c>
       <c r="L4">
-        <v>1.009106111240664</v>
+        <v>1.008593584247096</v>
       </c>
       <c r="M4">
-        <v>1.009064881190704</v>
+        <v>1.008546904162378</v>
       </c>
       <c r="N4">
-        <v>1.023320448473356</v>
+        <v>1.023319199768858</v>
       </c>
       <c r="O4">
-        <v>1.022117955738541</v>
+        <v>1.022076360174377</v>
       </c>
       <c r="P4">
-        <v>1.021423061652893</v>
+        <v>1.021381436758713</v>
       </c>
       <c r="Q4">
-        <v>1.009585792803257</v>
+        <v>1.008840240520714</v>
       </c>
       <c r="R4">
-        <v>1.022101810803212</v>
+        <v>1.021936385247691</v>
       </c>
       <c r="S4">
-        <v>1.010090883981644</v>
+        <v>1.009504806491458</v>
       </c>
       <c r="T4">
-        <v>1.009048942436122</v>
+        <v>1.008279578263803</v>
       </c>
       <c r="U4">
-        <v>1.01077152200823</v>
+        <v>1.010069852443143</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -637,61 +637,61 @@
         <v>1.03</v>
       </c>
       <c r="C5">
-        <v>1.023032344977129</v>
+        <v>1.02302480189348</v>
       </c>
       <c r="D5">
-        <v>1.018460687785299</v>
+        <v>1.018380055808593</v>
       </c>
       <c r="E5">
-        <v>1.010792633532484</v>
+        <v>1.010599498094862</v>
       </c>
       <c r="F5">
-        <v>1.010388202463306</v>
+        <v>1.010189957966755</v>
       </c>
       <c r="G5">
-        <v>1.010112151498272</v>
+        <v>1.009909244707296</v>
       </c>
       <c r="H5">
-        <v>1.009793937534579</v>
+        <v>1.0095909452662</v>
       </c>
       <c r="I5">
-        <v>1.009576947010703</v>
+        <v>1.009362074790257</v>
       </c>
       <c r="J5">
-        <v>1.009607181232206</v>
+        <v>1.009392335827987</v>
       </c>
       <c r="K5">
-        <v>1.009386610135802</v>
+        <v>1.009169079805256</v>
       </c>
       <c r="L5">
-        <v>1.009111669850853</v>
+        <v>1.008887744295604</v>
       </c>
       <c r="M5">
-        <v>1.009070450157617</v>
+        <v>1.008843804828139</v>
       </c>
       <c r="N5">
-        <v>1.023321936726942</v>
+        <v>1.023318071368558</v>
       </c>
       <c r="O5">
-        <v>1.022119705290602</v>
+        <v>1.021994655427625</v>
       </c>
       <c r="P5">
-        <v>1.021424960830191</v>
+        <v>1.021299822802728</v>
       </c>
       <c r="Q5">
-        <v>1.009591233911687</v>
+        <v>1.00925100026342</v>
       </c>
       <c r="R5">
-        <v>1.022103560327637</v>
+        <v>1.021605833732119</v>
       </c>
       <c r="S5">
-        <v>1.010096196201459</v>
+        <v>1.009767965362207</v>
       </c>
       <c r="T5">
-        <v>1.00905451131507</v>
+        <v>1.008702409532029</v>
       </c>
       <c r="U5">
-        <v>1.01077666748707</v>
+        <v>1.010583535101881</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -702,61 +702,61 @@
         <v>1.03</v>
       </c>
       <c r="C6">
-        <v>1.023273096800445</v>
+        <v>1.023255897408271</v>
       </c>
       <c r="D6">
-        <v>1.018864800888</v>
+        <v>1.018677470037257</v>
       </c>
       <c r="E6">
-        <v>1.01145022836299</v>
+        <v>1.01100097937691</v>
       </c>
       <c r="F6">
-        <v>1.011058443968311</v>
+        <v>1.010598945241475</v>
       </c>
       <c r="G6">
-        <v>1.010791066721088</v>
+        <v>1.010322220216712</v>
       </c>
       <c r="H6">
-        <v>1.010483108715772</v>
+        <v>1.010014069526862</v>
       </c>
       <c r="I6">
-        <v>1.010274522940927</v>
+        <v>1.009792430196759</v>
       </c>
       <c r="J6">
-        <v>1.010302575830808</v>
+        <v>1.009820542210462</v>
       </c>
       <c r="K6">
-        <v>1.010088597794501</v>
+        <v>1.009603815441855</v>
       </c>
       <c r="L6">
-        <v>1.00982207728906</v>
+        <v>1.009330817851442</v>
       </c>
       <c r="M6">
-        <v>1.009782181811265</v>
+        <v>1.009288189964943</v>
       </c>
       <c r="N6">
-        <v>1.023512101775912</v>
+        <v>1.023512101776491</v>
       </c>
       <c r="O6">
-        <v>1.02234329669413</v>
+        <v>1.022343296695319</v>
       </c>
       <c r="P6">
-        <v>1.021667692889974</v>
+        <v>1.021667692891168</v>
       </c>
       <c r="Q6">
-        <v>1.010286617526135</v>
+        <v>1.009553515284103</v>
       </c>
       <c r="R6">
-        <v>1.022327148199412</v>
+        <v>1.02232714820717</v>
       </c>
       <c r="S6">
-        <v>1.010775100700422</v>
+        <v>1.010055310832054</v>
       </c>
       <c r="T6">
-        <v>1.009766231726512</v>
+        <v>1.009146843064988</v>
       </c>
       <c r="U6">
-        <v>1.011434251930491</v>
+        <v>1.010734228824527</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -767,61 +767,61 @@
         <v>1.03</v>
       </c>
       <c r="C7">
-        <v>1.023085262169533</v>
+        <v>1.023049280008193</v>
       </c>
       <c r="D7">
-        <v>1.018549485018173</v>
+        <v>1.018171546571496</v>
       </c>
       <c r="E7">
-        <v>1.010937099903137</v>
+        <v>1.01003305254734</v>
       </c>
       <c r="F7">
-        <v>1.010535446088573</v>
+        <v>1.009610826140785</v>
       </c>
       <c r="G7">
-        <v>1.010261299899466</v>
+        <v>1.009317920872699</v>
       </c>
       <c r="H7">
-        <v>1.009945338182877</v>
+        <v>1.009001563644202</v>
       </c>
       <c r="I7">
-        <v>1.00973019354211</v>
+        <v>1.008749454436298</v>
       </c>
       <c r="J7">
-        <v>1.009759948731113</v>
+        <v>1.008779331609329</v>
       </c>
       <c r="K7">
-        <v>1.009540825516052</v>
+        <v>1.008554690496652</v>
       </c>
       <c r="L7">
-        <v>1.009267734277196</v>
+        <v>1.008268606702818</v>
       </c>
       <c r="M7">
-        <v>1.009226805391169</v>
+        <v>1.008222199928343</v>
       </c>
       <c r="N7">
-        <v>1.023363719215656</v>
+        <v>1.02336119203823</v>
       </c>
       <c r="O7">
-        <v>1.02216882564266</v>
+        <v>1.022085561449552</v>
       </c>
       <c r="P7">
-        <v>1.021478283003358</v>
+        <v>1.02139496045465</v>
       </c>
       <c r="Q7">
-        <v>1.009743998997543</v>
+        <v>1.008132043769834</v>
       </c>
       <c r="R7">
-        <v>1.022152679903812</v>
+        <v>1.021821372549789</v>
       </c>
       <c r="S7">
-        <v>1.010245342246769</v>
+        <v>1.008797971285038</v>
       </c>
       <c r="T7">
-        <v>1.009210864078903</v>
+        <v>1.007954797676398</v>
       </c>
       <c r="U7">
-        <v>1.010921131575795</v>
+        <v>1.009639964370616</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -832,61 +832,61 @@
         <v>1.03</v>
       </c>
       <c r="C8">
-        <v>1.022630780272726</v>
+        <v>1.022599087587895</v>
       </c>
       <c r="D8">
-        <v>1.01778733211316</v>
+        <v>1.017462031105671</v>
       </c>
       <c r="E8">
-        <v>1.00969766887615</v>
+        <v>1.008920937441804</v>
       </c>
       <c r="F8">
-        <v>1.009272207662286</v>
+        <v>1.008479974281017</v>
       </c>
       <c r="G8">
-        <v>1.008981733264197</v>
+        <v>1.008175380509967</v>
       </c>
       <c r="H8">
-        <v>1.008646464617772</v>
+        <v>1.007839758045094</v>
       </c>
       <c r="I8">
-        <v>1.008415493433572</v>
+        <v>1.007594465417679</v>
       </c>
       <c r="J8">
-        <v>1.008449355101644</v>
+        <v>1.007628432572822</v>
       </c>
       <c r="K8">
-        <v>1.008217819842967</v>
+        <v>1.007394043328788</v>
       </c>
       <c r="L8">
-        <v>1.007928877468999</v>
+        <v>1.007098480669374</v>
       </c>
       <c r="M8">
-        <v>1.007885455614795</v>
+        <v>1.007052299449739</v>
       </c>
       <c r="N8">
-        <v>1.023005156338313</v>
+        <v>1.02300117972796</v>
       </c>
       <c r="O8">
-        <v>1.021747409679758</v>
+        <v>1.021622196403153</v>
       </c>
       <c r="P8">
-        <v>1.021020875965341</v>
+        <v>1.020895570470776</v>
       </c>
       <c r="Q8">
-        <v>1.008433426069647</v>
+        <v>1.007234473764515</v>
       </c>
       <c r="R8">
-        <v>1.021731270597415</v>
+        <v>1.021233243453742</v>
       </c>
       <c r="S8">
-        <v>1.008965795822985</v>
+        <v>1.007781620116075</v>
       </c>
       <c r="T8">
-        <v>1.007869535489912</v>
+        <v>1.006910708549217</v>
       </c>
       <c r="U8">
-        <v>1.009681720126326</v>
+        <v>1.008273737375279</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -897,61 +897,61 @@
         <v>1.03</v>
       </c>
       <c r="C9">
-        <v>1.021363395167066</v>
+        <v>1.02132709904349</v>
       </c>
       <c r="D9">
-        <v>1.015644861136213</v>
+        <v>1.015310493493901</v>
       </c>
       <c r="E9">
-        <v>1.006199090528654</v>
+        <v>1.005407346242882</v>
       </c>
       <c r="F9">
-        <v>1.005707880068399</v>
+        <v>1.004910623174902</v>
       </c>
       <c r="G9">
-        <v>1.005372312444564</v>
+        <v>1.004570110067247</v>
       </c>
       <c r="H9">
-        <v>1.00498372247808</v>
+        <v>1.004181124467152</v>
       </c>
       <c r="I9">
-        <v>1.004698221098066</v>
+        <v>1.003807358148684</v>
       </c>
       <c r="J9">
-        <v>1.004743428567433</v>
+        <v>1.003852690263196</v>
       </c>
       <c r="K9">
-        <v>1.004474964022374</v>
+        <v>1.003567965425974</v>
       </c>
       <c r="L9">
-        <v>1.004135879433539</v>
+        <v>1.003190088728251</v>
       </c>
       <c r="M9">
-        <v>1.004082849790051</v>
+        <v>1.003120542595835</v>
       </c>
       <c r="N9">
-        <v>1.022010969472218</v>
+        <v>1.02200195855004</v>
       </c>
       <c r="O9">
-        <v>1.020580323946099</v>
+        <v>1.020328076609923</v>
       </c>
       <c r="P9">
-        <v>1.019754784223468</v>
+        <v>1.019502326328291</v>
       </c>
       <c r="Q9">
-        <v>1.004727558072657</v>
+        <v>1.003457355467199</v>
       </c>
       <c r="R9">
-        <v>1.02056420329854</v>
+        <v>1.019561879469991</v>
       </c>
       <c r="S9">
-        <v>1.005356432016209</v>
+        <v>1.004428246822216</v>
       </c>
       <c r="T9">
-        <v>1.003940932901547</v>
+        <v>1.002212872875783</v>
       </c>
       <c r="U9">
-        <v>1.006183197040868</v>
+        <v>1.005139279870237</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -962,61 +962,61 @@
         <v>1.03</v>
       </c>
       <c r="C10">
-        <v>1.016802362852875</v>
+        <v>1.016711825345493</v>
       </c>
       <c r="D10">
-        <v>1.008033741417685</v>
+        <v>1.007376494128347</v>
       </c>
       <c r="E10">
-        <v>0.9938730620146456</v>
+        <v>0.9923528122019485</v>
       </c>
       <c r="F10">
-        <v>0.9931510739316922</v>
+        <v>0.9915935287109746</v>
       </c>
       <c r="G10">
-        <v>0.9926572391312937</v>
+        <v>0.9910658154278791</v>
       </c>
       <c r="H10">
-        <v>0.9920814882622695</v>
+        <v>0.9904889697845853</v>
       </c>
       <c r="I10">
-        <v>0.9916308499243941</v>
+        <v>0.9900404704033</v>
       </c>
       <c r="J10">
-        <v>0.9917158853351832</v>
+        <v>0.9901257933637626</v>
       </c>
       <c r="K10">
-        <v>0.9913243013948994</v>
+        <v>0.9897254125419274</v>
       </c>
       <c r="L10">
-        <v>0.9908249013032678</v>
+        <v>0.9892056279367476</v>
       </c>
       <c r="M10">
-        <v>0.9907448876439935</v>
+        <v>0.989117124393659</v>
       </c>
       <c r="N10">
-        <v>1.018471851288541</v>
+        <v>1.018464376418338</v>
       </c>
       <c r="O10">
-        <v>1.016441188574724</v>
+        <v>1.016270970584856</v>
       </c>
       <c r="P10">
-        <v>1.015272061620074</v>
+        <v>1.015101643210832</v>
       </c>
       <c r="Q10">
-        <v>0.9917002206178736</v>
+        <v>0.9897253625033329</v>
       </c>
       <c r="R10">
-        <v>1.016425133307166</v>
+        <v>1.015754402882731</v>
       </c>
       <c r="S10">
-        <v>0.9926415595447645</v>
+        <v>0.9901472400161411</v>
       </c>
       <c r="T10">
-        <v>0.9904732961581285</v>
+        <v>0.988457390970684</v>
       </c>
       <c r="U10">
-        <v>0.9937300072087434</v>
+        <v>0.9910426106927058</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1027,61 +1027,61 @@
         <v>1.03</v>
       </c>
       <c r="C11">
-        <v>1.012588838769329</v>
+        <v>1.012482774666418</v>
       </c>
       <c r="D11">
-        <v>1.001191568913407</v>
+        <v>1.000527819163288</v>
       </c>
       <c r="E11">
-        <v>0.9829796157060122</v>
+        <v>0.9814713527145551</v>
       </c>
       <c r="F11">
-        <v>0.9820510333933109</v>
+        <v>0.9805046965670281</v>
       </c>
       <c r="G11">
-        <v>0.9814155281145883</v>
+        <v>0.9798346910784728</v>
       </c>
       <c r="H11">
-        <v>0.9806722242949931</v>
+        <v>0.9790900177944137</v>
       </c>
       <c r="I11">
-        <v>0.9801050860751827</v>
+        <v>0.9784914334243489</v>
       </c>
       <c r="J11">
-        <v>0.9802257719967736</v>
+        <v>0.9786124715381187</v>
       </c>
       <c r="K11">
-        <v>0.9797317127135053</v>
+        <v>0.9781066200043835</v>
       </c>
       <c r="L11">
-        <v>0.9791074610604699</v>
+        <v>0.9774550138803533</v>
       </c>
       <c r="M11">
-        <v>0.9790113072538538</v>
+        <v>0.9773474582336817</v>
       </c>
       <c r="N11">
-        <v>1.015240276294989</v>
+        <v>1.015214092536266</v>
       </c>
       <c r="O11">
-        <v>1.012681064882454</v>
+        <v>1.012203458501552</v>
       </c>
       <c r="P11">
-        <v>1.011209271566258</v>
+        <v>1.010730957037989</v>
       </c>
       <c r="Q11">
-        <v>0.9802102887723492</v>
+        <v>0.9779458737311366</v>
       </c>
       <c r="R11">
-        <v>1.012665069008192</v>
+        <v>1.010790107388613</v>
       </c>
       <c r="S11">
-        <v>0.9814000260972882</v>
+        <v>0.9789057009631953</v>
       </c>
       <c r="T11">
-        <v>0.9789958432125917</v>
+        <v>0.9768113065354642</v>
       </c>
       <c r="U11">
-        <v>0.9829640889830576</v>
+        <v>0.9808066383507729</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1092,61 +1092,61 @@
         <v>1.03</v>
       </c>
       <c r="C12">
-        <v>1.005291285247945</v>
+        <v>1.005009013791476</v>
       </c>
       <c r="D12">
-        <v>0.9893172438736818</v>
+        <v>0.987899540216739</v>
       </c>
       <c r="E12">
-        <v>0.9640868060587174</v>
+        <v>0.9609671724810916</v>
       </c>
       <c r="F12">
-        <v>0.9628100180462619</v>
+        <v>0.9596484323175846</v>
       </c>
       <c r="G12">
-        <v>0.9619345460057833</v>
+        <v>0.9587356046986832</v>
       </c>
       <c r="H12">
-        <v>0.9609130906788442</v>
+        <v>0.9577103911307245</v>
       </c>
       <c r="I12">
-        <v>0.9601249750334161</v>
+        <v>0.9567374605263895</v>
       </c>
       <c r="J12">
-        <v>0.9603048914670528</v>
+        <v>0.9569183358487727</v>
       </c>
       <c r="K12">
-        <v>0.9596316427113677</v>
+        <v>0.956222927563005</v>
       </c>
       <c r="L12">
-        <v>0.9587784673460167</v>
+        <v>0.9553193525351332</v>
       </c>
       <c r="M12">
-        <v>0.9586463159631599</v>
+        <v>0.9551665179820705</v>
       </c>
       <c r="N12">
-        <v>1.009783371471103</v>
+        <v>1.009747227326449</v>
       </c>
       <c r="O12">
-        <v>1.006368473770559</v>
+        <v>1.005835892228512</v>
       </c>
       <c r="P12">
-        <v>1.004406674851279</v>
+        <v>1.003873037441537</v>
       </c>
       <c r="Q12">
-        <v>0.9602897229042833</v>
+        <v>0.9548692627713272</v>
       </c>
       <c r="R12">
-        <v>1.006352577607268</v>
+        <v>1.004283176480023</v>
       </c>
       <c r="S12">
-        <v>0.9617877525498503</v>
+        <v>0.9576510331788527</v>
       </c>
       <c r="T12">
-        <v>0.9586311735985356</v>
+        <v>0.9542137472449568</v>
       </c>
       <c r="U12">
-        <v>0.9639402734214186</v>
+        <v>0.9593404722985189</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1157,61 +1157,61 @@
         <v>1.03</v>
       </c>
       <c r="C13">
-        <v>0.999192638821529</v>
+        <v>0.9987377913338281</v>
       </c>
       <c r="D13">
-        <v>0.9795442061328651</v>
+        <v>0.9775327710641171</v>
       </c>
       <c r="E13">
-        <v>0.9487058783336341</v>
+        <v>0.9443785680777389</v>
       </c>
       <c r="F13">
-        <v>0.9471586229165643</v>
+        <v>0.942735700859437</v>
       </c>
       <c r="G13">
-        <v>0.9460989338061557</v>
+        <v>0.941590340051615</v>
       </c>
       <c r="H13">
-        <v>0.9448538168486762</v>
+        <v>0.940338759443089</v>
       </c>
       <c r="I13">
-        <v>0.9438568632049126</v>
+        <v>0.9392092997053345</v>
       </c>
       <c r="J13">
-        <v>0.9440844360114299</v>
+        <v>0.9394384405444979</v>
       </c>
       <c r="K13">
-        <v>0.9432640920251696</v>
+        <v>0.9385703882955626</v>
       </c>
       <c r="L13">
-        <v>0.9422197866336002</v>
+        <v>0.9374163171939207</v>
       </c>
       <c r="M13">
-        <v>0.9420557486453598</v>
+        <v>0.9372068283607066</v>
       </c>
       <c r="N13">
-        <v>1.005320574659114</v>
+        <v>1.005274161381137</v>
       </c>
       <c r="O13">
-        <v>1.001195306239324</v>
+        <v>1.000606799797854</v>
       </c>
       <c r="P13">
-        <v>0.9988502741275889</v>
+        <v>0.9982603675028539</v>
       </c>
       <c r="Q13">
-        <v>0.9440695236599941</v>
+        <v>0.9380535656506952</v>
       </c>
       <c r="R13">
-        <v>1.001053070224063</v>
+        <v>0.9987824965162884</v>
       </c>
       <c r="S13">
-        <v>0.9460839896345794</v>
+        <v>0.9393646996381034</v>
       </c>
       <c r="T13">
-        <v>0.9419064821813122</v>
+        <v>0.9349703149021142</v>
       </c>
       <c r="U13">
-        <v>0.9485574522450069</v>
+        <v>0.9427226076182712</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1222,61 +1222,61 @@
         <v>1.03</v>
       </c>
       <c r="C14">
-        <v>0.9986297414635703</v>
+        <v>0.9981327963057236</v>
       </c>
       <c r="D14">
-        <v>0.9786952898229836</v>
+        <v>0.9765162210460857</v>
       </c>
       <c r="E14">
-        <v>0.9474195197110752</v>
+        <v>0.9427395580076526</v>
       </c>
       <c r="F14">
-        <v>0.9458468098485923</v>
+        <v>0.9410702970427287</v>
       </c>
       <c r="G14">
-        <v>0.9447696707018077</v>
+        <v>0.9399068075166912</v>
       </c>
       <c r="H14">
-        <v>0.9435039071907052</v>
+        <v>0.9386339531105692</v>
       </c>
       <c r="I14">
-        <v>0.9425012627701569</v>
+        <v>0.9374748291118029</v>
       </c>
       <c r="J14">
-        <v>0.9427332260974679</v>
+        <v>0.9377085141931842</v>
       </c>
       <c r="K14">
-        <v>0.9419023971447245</v>
+        <v>0.936832521944934</v>
       </c>
       <c r="L14">
-        <v>0.9408478691317274</v>
+        <v>0.9356748121285342</v>
       </c>
       <c r="M14">
-        <v>0.9406840591855485</v>
+        <v>0.9354685128988517</v>
       </c>
       <c r="N14">
-        <v>1.004901796579519</v>
+        <v>1.004873754376655</v>
       </c>
       <c r="O14">
-        <v>1.000714956550865</v>
+        <v>1.000354169855862</v>
       </c>
       <c r="P14">
-        <v>0.9983346761873054</v>
+        <v>0.9979730180529768</v>
       </c>
       <c r="Q14">
-        <v>0.9427183350891621</v>
+        <v>0.9358994308534326</v>
       </c>
       <c r="R14">
-        <v>1.000572667242923</v>
+        <v>0.9991847761858649</v>
       </c>
       <c r="S14">
-        <v>0.9447547475266997</v>
+        <v>0.9376770042739817</v>
       </c>
       <c r="T14">
-        <v>0.9406692005469109</v>
+        <v>0.9335130398442163</v>
       </c>
       <c r="U14">
-        <v>0.9474045546817551</v>
+        <v>0.9409404215658662</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1287,61 +1287,61 @@
         <v>1.03</v>
       </c>
       <c r="C15">
-        <v>0.9991013373374988</v>
+        <v>0.9986579036317065</v>
       </c>
       <c r="D15">
-        <v>0.9794472496273685</v>
+        <v>0.9774808178050718</v>
       </c>
       <c r="E15">
-        <v>0.9485984038134813</v>
+        <v>0.9443660965707368</v>
       </c>
       <c r="F15">
-        <v>0.9470466488740856</v>
+        <v>0.9427411728142285</v>
       </c>
       <c r="G15">
-        <v>0.9459838752675608</v>
+        <v>0.9416132114507911</v>
       </c>
       <c r="H15">
-        <v>0.9447351098300686</v>
+        <v>0.9403581632159033</v>
       </c>
       <c r="I15">
-        <v>0.9437467309404122</v>
+        <v>0.9391834551914862</v>
       </c>
       <c r="J15">
-        <v>0.9439750720056165</v>
+        <v>0.9394133395958276</v>
       </c>
       <c r="K15">
-        <v>0.9431552117952808</v>
+        <v>0.938548887507062</v>
       </c>
       <c r="L15">
-        <v>0.9421147006592587</v>
+        <v>0.9374060149564929</v>
       </c>
       <c r="M15">
-        <v>0.9419530944998664</v>
+        <v>0.9372020991826759</v>
       </c>
       <c r="N15">
-        <v>1.005246053913256</v>
+        <v>1.005192369983939</v>
       </c>
       <c r="O15">
-        <v>1.001150673459158</v>
+        <v>1.000471428706037</v>
       </c>
       <c r="P15">
-        <v>0.9987991910981058</v>
+        <v>0.9981183256356716</v>
       </c>
       <c r="Q15">
-        <v>0.9439601613816473</v>
+        <v>0.9377484056140301</v>
       </c>
       <c r="R15">
-        <v>1.001134859714451</v>
+        <v>0.998514562355555</v>
       </c>
       <c r="S15">
-        <v>0.9459689329133998</v>
+        <v>0.9399522658920987</v>
       </c>
       <c r="T15">
-        <v>0.9419382158141837</v>
+        <v>0.9352503723074369</v>
       </c>
       <c r="U15">
-        <v>0.9485834201613526</v>
+        <v>0.9425701515771796</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1352,61 +1352,61 @@
         <v>1.03</v>
       </c>
       <c r="C16">
-        <v>0.9991154903043551</v>
+        <v>0.998699398978526</v>
       </c>
       <c r="D16">
-        <v>0.9794698238862778</v>
+        <v>0.9776218012631885</v>
       </c>
       <c r="E16">
-        <v>0.9486338037481201</v>
+        <v>0.9446550720291981</v>
       </c>
       <c r="F16">
-        <v>0.9470826784383142</v>
+        <v>0.943025697772744</v>
       </c>
       <c r="G16">
-        <v>0.9460203364730752</v>
+        <v>0.9418934203814534</v>
       </c>
       <c r="H16">
-        <v>0.9447720817728871</v>
+        <v>0.9406392372248302</v>
       </c>
       <c r="I16">
-        <v>0.9437841314116513</v>
+        <v>0.9395230255972066</v>
       </c>
       <c r="J16">
-        <v>0.9440123636415394</v>
+        <v>0.9397526980363057</v>
       </c>
       <c r="K16">
-        <v>0.9431928329934018</v>
+        <v>0.9388859328028106</v>
       </c>
       <c r="L16">
-        <v>0.9421527429997532</v>
+        <v>0.937736829174897</v>
       </c>
       <c r="M16">
-        <v>0.9419912030542014</v>
+        <v>0.9375300405094651</v>
       </c>
       <c r="N16">
-        <v>1.005253026490207</v>
+        <v>1.005194716189954</v>
       </c>
       <c r="O16">
-        <v>1.001117812489593</v>
+        <v>1.00039099613441</v>
       </c>
       <c r="P16">
-        <v>0.99876708677496</v>
+        <v>0.998038536618166</v>
       </c>
       <c r="Q16">
-        <v>0.943997452428528</v>
+        <v>0.9387844001875572</v>
       </c>
       <c r="R16">
-        <v>1.000975567880773</v>
+        <v>0.998168071271893</v>
       </c>
       <c r="S16">
-        <v>0.9460053935429887</v>
+        <v>0.9400926190221198</v>
       </c>
       <c r="T16">
-        <v>0.941976323766572</v>
+        <v>0.9354369309870125</v>
       </c>
       <c r="U16">
-        <v>0.9486188195368294</v>
+        <v>0.9428596928011719</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1417,61 +1417,61 @@
         <v>1.03</v>
       </c>
       <c r="C17">
-        <v>0.9991769187130788</v>
+        <v>0.9986046581550297</v>
       </c>
       <c r="D17">
-        <v>0.97956780839554</v>
+        <v>0.9770465374760666</v>
       </c>
       <c r="E17">
-        <v>0.9487874648591721</v>
+        <v>0.9433678261988624</v>
       </c>
       <c r="F17">
-        <v>0.9472390728564094</v>
+        <v>0.9417217808842819</v>
       </c>
       <c r="G17">
-        <v>0.9461786047055659</v>
+        <v>0.9405742184638808</v>
       </c>
       <c r="H17">
-        <v>0.9449325671840161</v>
+        <v>0.9393201323701914</v>
       </c>
       <c r="I17">
-        <v>0.9439464770510658</v>
+        <v>0.9381650885239089</v>
       </c>
       <c r="J17">
-        <v>0.9441742368136959</v>
+        <v>0.9383948019027646</v>
       </c>
       <c r="K17">
-        <v>0.9433561368300762</v>
+        <v>0.9375368202469755</v>
       </c>
       <c r="L17">
-        <v>0.9423178750583359</v>
+        <v>0.9364087334870905</v>
       </c>
       <c r="M17">
-        <v>0.9421566225539616</v>
+        <v>0.9362109109019984</v>
       </c>
       <c r="N17">
-        <v>1.005297486013602</v>
+        <v>1.005243227461577</v>
       </c>
       <c r="O17">
-        <v>1.001168817478008</v>
+        <v>1.000488264479699</v>
       </c>
       <c r="P17">
-        <v>0.9988218388827843</v>
+        <v>0.9981396651739445</v>
       </c>
       <c r="Q17">
-        <v>0.944159323043805</v>
+        <v>0.9361612460822412</v>
       </c>
       <c r="R17">
-        <v>1.001026578525464</v>
+        <v>0.9983987072504698</v>
       </c>
       <c r="S17">
-        <v>0.9461636592755426</v>
+        <v>0.9383460674545707</v>
       </c>
       <c r="T17">
-        <v>0.9421417406534374</v>
+        <v>0.9345401350771381</v>
       </c>
       <c r="U17">
-        <v>0.948772478220717</v>
+        <v>0.9404309536729525</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1482,61 +1482,61 @@
         <v>1.03</v>
       </c>
       <c r="C18">
-        <v>1.005023339728152</v>
+        <v>1.004534830888391</v>
       </c>
       <c r="D18">
-        <v>0.9888860613162325</v>
+        <v>0.9864983978384183</v>
       </c>
       <c r="E18">
-        <v>0.9634059795865239</v>
+        <v>0.9581752280523791</v>
       </c>
       <c r="F18">
-        <v>0.9621221585608504</v>
+        <v>0.95680276415192</v>
       </c>
       <c r="G18">
-        <v>0.9612430764305581</v>
+        <v>0.9558443296536079</v>
       </c>
       <c r="H18">
-        <v>0.9602116427128371</v>
+        <v>0.9548064783740231</v>
       </c>
       <c r="I18">
-        <v>0.9594050653084628</v>
+        <v>0.953742339076379</v>
       </c>
       <c r="J18">
-        <v>0.9595871096159214</v>
+        <v>0.9539260029299139</v>
       </c>
       <c r="K18">
-        <v>0.9589074207783873</v>
+        <v>0.9532023262203336</v>
       </c>
       <c r="L18">
-        <v>0.9580460170812324</v>
+        <v>0.9522400626066423</v>
       </c>
       <c r="M18">
-        <v>0.9579125718947352</v>
+        <v>0.9520649612006401</v>
       </c>
       <c r="N18">
-        <v>1.009585311052824</v>
+        <v>1.009531890073061</v>
       </c>
       <c r="O18">
-        <v>1.006140152316456</v>
+        <v>1.005381077023319</v>
       </c>
       <c r="P18">
-        <v>1.004161024335809</v>
+        <v>1.003400430273486</v>
       </c>
       <c r="Q18">
-        <v>0.9595719523909255</v>
+        <v>0.9510236977069273</v>
       </c>
       <c r="R18">
-        <v>1.006124259759633</v>
+        <v>1.003169620307694</v>
       </c>
       <c r="S18">
-        <v>0.961227893048623</v>
+        <v>0.9537928678409018</v>
       </c>
       <c r="T18">
-        <v>0.9578974411200164</v>
+        <v>0.9501447475846725</v>
       </c>
       <c r="U18">
-        <v>0.9631275068543628</v>
+        <v>0.9557099211639819</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1547,61 +1547,61 @@
         <v>1.03</v>
       </c>
       <c r="C19">
-        <v>1.014640504004088</v>
+        <v>1.014240456569193</v>
       </c>
       <c r="D19">
-        <v>1.004455795877137</v>
+        <v>1.001985347122213</v>
       </c>
       <c r="E19">
-        <v>0.9881124899111815</v>
+        <v>0.9825060917573073</v>
       </c>
       <c r="F19">
-        <v>0.987284093165966</v>
+        <v>0.981566854047879</v>
       </c>
       <c r="G19">
-        <v>0.9867172878390323</v>
+        <v>0.9808997587228475</v>
       </c>
       <c r="H19">
-        <v>0.9860552362786432</v>
+        <v>0.9802331548905583</v>
       </c>
       <c r="I19">
-        <v>0.9855331962928527</v>
+        <v>0.9794672011534585</v>
       </c>
       <c r="J19">
-        <v>0.9856366011977469</v>
+        <v>0.9795718235400499</v>
       </c>
       <c r="K19">
-        <v>0.9851894396592865</v>
+        <v>0.97906027846354</v>
       </c>
       <c r="L19">
-        <v>0.9846190102842574</v>
+        <v>0.978338473977665</v>
       </c>
       <c r="M19">
-        <v>0.9845278044067146</v>
+        <v>0.9781835235768156</v>
       </c>
       <c r="N19">
-        <v>1.016816657402483</v>
+        <v>1.016777103090166</v>
       </c>
       <c r="O19">
-        <v>1.014513099432663</v>
+        <v>1.013774849831582</v>
       </c>
       <c r="P19">
-        <v>1.013187703129871</v>
+        <v>1.012448467811389</v>
       </c>
       <c r="Q19">
-        <v>0.9856210325061929</v>
+        <v>0.9772996810423099</v>
       </c>
       <c r="R19">
-        <v>1.014497074620371</v>
+        <v>1.011582407504162</v>
       </c>
       <c r="S19">
-        <v>0.9867017020774175</v>
+        <v>0.9782198958966697</v>
       </c>
       <c r="T19">
-        <v>0.9842546841082818</v>
+        <v>0.974939899077974</v>
       </c>
       <c r="U19">
-        <v>0.9878402536292518</v>
+        <v>0.9798308483556265</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1612,61 +1612,61 @@
         <v>1.03</v>
       </c>
       <c r="C20">
-        <v>1.017021457375059</v>
+        <v>1.016720706440919</v>
       </c>
       <c r="D20">
-        <v>1.00841832642861</v>
+        <v>1.006360345583179</v>
       </c>
       <c r="E20">
-        <v>0.9945125769946667</v>
+        <v>0.9897826708085163</v>
       </c>
       <c r="F20">
-        <v>0.9938013355766536</v>
+        <v>0.9889947467453553</v>
       </c>
       <c r="G20">
-        <v>0.9933148706152393</v>
+        <v>0.988438925420245</v>
       </c>
       <c r="H20">
-        <v>0.9927478360822504</v>
+        <v>0.9878685713435873</v>
       </c>
       <c r="I20">
-        <v>0.9923263173895136</v>
+        <v>0.987226532372573</v>
       </c>
       <c r="J20">
-        <v>0.9924094915680923</v>
+        <v>0.9873106211155417</v>
       </c>
       <c r="K20">
-        <v>0.9920288927954519</v>
+        <v>0.98687850476116</v>
       </c>
       <c r="L20">
-        <v>0.991549568852938</v>
+        <v>0.986277782582953</v>
       </c>
       <c r="M20">
-        <v>0.9914762058275416</v>
+        <v>0.9861532090487753</v>
       </c>
       <c r="N20">
-        <v>1.018637431352431</v>
+        <v>1.018591224771914</v>
       </c>
       <c r="O20">
-        <v>1.016634328864176</v>
+        <v>1.015725099460699</v>
       </c>
       <c r="P20">
-        <v>1.015480983800037</v>
+        <v>1.014570697464714</v>
       </c>
       <c r="Q20">
-        <v>0.9923938158948772</v>
+        <v>0.9854610556436039</v>
       </c>
       <c r="R20">
-        <v>1.016618270545857</v>
+        <v>1.013009250367594</v>
       </c>
       <c r="S20">
-        <v>0.9932991806410464</v>
+        <v>0.986591532053674</v>
       </c>
       <c r="T20">
-        <v>0.9914605448961062</v>
+        <v>0.98376114866292</v>
       </c>
       <c r="U20">
-        <v>0.9942419020061054</v>
+        <v>0.9867174371258072</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1677,61 +1677,61 @@
         <v>1.03</v>
       </c>
       <c r="C21">
-        <v>1.019494017828853</v>
+        <v>1.019214948684147</v>
       </c>
       <c r="D21">
-        <v>1.012532896215236</v>
+        <v>1.010424987172349</v>
       </c>
       <c r="E21">
-        <v>1.001163703961013</v>
+        <v>0.996265216698521</v>
       </c>
       <c r="F21">
-        <v>1.000576706198582</v>
+        <v>0.9956130252535789</v>
       </c>
       <c r="G21">
-        <v>1.00017544616216</v>
+        <v>0.9951528015592596</v>
       </c>
       <c r="H21">
-        <v>0.999709174206125</v>
+        <v>0.9946836398307588</v>
       </c>
       <c r="I21">
-        <v>0.9993706258661331</v>
+        <v>0.9940279738799883</v>
       </c>
       <c r="J21">
-        <v>0.9994323577530153</v>
+        <v>0.9940905456063903</v>
       </c>
       <c r="K21">
-        <v>0.9991165812963029</v>
+        <v>0.993723892918601</v>
       </c>
       <c r="L21">
-        <v>0.9987200509227273</v>
+        <v>0.9932071875801385</v>
       </c>
       <c r="M21">
-        <v>0.998659708543177</v>
+        <v>0.9930960579878894</v>
       </c>
       <c r="N21">
-        <v>1.020550319408322</v>
+        <v>1.020498826812595</v>
       </c>
       <c r="O21">
-        <v>1.01886919354919</v>
+        <v>1.017790533949064</v>
       </c>
       <c r="P21">
-        <v>1.017900222117251</v>
+        <v>1.016820507367092</v>
       </c>
       <c r="Q21">
-        <v>0.9994165711496283</v>
+        <v>0.9913123303757265</v>
       </c>
       <c r="R21">
-        <v>1.01885309992991</v>
+        <v>1.014547517001705</v>
       </c>
       <c r="S21">
-        <v>1.000159647821269</v>
+        <v>0.9935831161598898</v>
       </c>
       <c r="T21">
-        <v>0.9986439341442244</v>
+        <v>0.99072147660779</v>
       </c>
       <c r="U21">
-        <v>1.001021464441422</v>
+        <v>0.9934934053114188</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1742,61 +1742,61 @@
         <v>1.03</v>
       </c>
       <c r="C22">
-        <v>1.020387907092537</v>
+        <v>1.020206833292289</v>
       </c>
       <c r="D22">
-        <v>1.014018869210015</v>
+        <v>1.012543385164436</v>
       </c>
       <c r="E22">
-        <v>1.003565790778334</v>
+        <v>1.000110769504221</v>
       </c>
       <c r="F22">
-        <v>1.003019350023675</v>
+        <v>0.9995108069481214</v>
       </c>
       <c r="G22">
-        <v>1.002644738495079</v>
+        <v>0.9990876538100957</v>
       </c>
       <c r="H22">
-        <v>1.002215448495906</v>
+        <v>0.9986564561434546</v>
       </c>
       <c r="I22">
-        <v>1.00191699082497</v>
+        <v>0.9981134663582676</v>
       </c>
       <c r="J22">
-        <v>1.001970853814235</v>
+        <v>0.9981678960074742</v>
       </c>
       <c r="K22">
-        <v>1.001678866129812</v>
+        <v>0.9978368860164273</v>
       </c>
       <c r="L22">
-        <v>1.001312718191562</v>
+        <v>0.9973783299491263</v>
       </c>
       <c r="M22">
-        <v>1.001257154001173</v>
+        <v>0.9972836383671657</v>
       </c>
       <c r="N22">
-        <v>1.021247445476572</v>
+        <v>1.021202903668786</v>
       </c>
       <c r="O22">
-        <v>1.019685351916267</v>
+        <v>1.018697866193399</v>
       </c>
       <c r="P22">
-        <v>1.018784541653293</v>
+        <v>1.017796157131988</v>
       </c>
       <c r="Q22">
-        <v>1.001955027113856</v>
+        <v>0.9959398219549739</v>
       </c>
       <c r="R22">
-        <v>1.019669245405301</v>
+        <v>1.01572494281015</v>
       </c>
       <c r="S22">
-        <v>1.002502662935864</v>
+        <v>0.9976555181906851</v>
       </c>
       <c r="T22">
-        <v>1.00124133857409</v>
+        <v>0.9954530890526206</v>
       </c>
       <c r="U22">
-        <v>1.003549938895375</v>
+        <v>0.9988108122067787</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1807,61 +1807,61 @@
         <v>1.03</v>
       </c>
       <c r="C23">
-        <v>1.020688606726456</v>
+        <v>1.02054262197399</v>
       </c>
       <c r="D23">
-        <v>1.014519540691325</v>
+        <v>1.013289246789613</v>
       </c>
       <c r="E23">
-        <v>1.004376027946628</v>
+        <v>1.001486175411977</v>
       </c>
       <c r="F23">
-        <v>1.003850062981376</v>
+        <v>1.000917601146358</v>
       </c>
       <c r="G23">
-        <v>1.003490659920631</v>
+        <v>1.000519560799574</v>
       </c>
       <c r="H23">
-        <v>1.003073884773666</v>
+        <v>1.000101231437502</v>
       </c>
       <c r="I23">
-        <v>1.002765212790965</v>
+        <v>0.9996063609546163</v>
       </c>
       <c r="J23">
-        <v>1.002816416106022</v>
+        <v>0.9996580261270288</v>
       </c>
       <c r="K23">
-        <v>1.002529821103487</v>
+        <v>0.99934352999339</v>
       </c>
       <c r="L23">
-        <v>1.002167575485418</v>
+        <v>0.998915339674924</v>
       </c>
       <c r="M23">
-        <v>1.002110899923668</v>
+        <v>0.998830782035843</v>
       </c>
       <c r="N23">
-        <v>1.021482550812523</v>
+        <v>1.021456364852239</v>
       </c>
       <c r="O23">
-        <v>1.019960811448616</v>
+        <v>1.019322807257644</v>
       </c>
       <c r="P23">
-        <v>1.019083109065594</v>
+        <v>1.018444539036162</v>
       </c>
       <c r="Q23">
-        <v>1.002800576049505</v>
+        <v>0.9978319441769655</v>
       </c>
       <c r="R23">
-        <v>1.019944700586609</v>
+        <v>1.017403221193763</v>
       </c>
       <c r="S23">
-        <v>1.003474809215203</v>
+        <v>0.9994801681804111</v>
       </c>
       <c r="T23">
-        <v>1.001968765327675</v>
+        <v>0.9973982733342519</v>
       </c>
       <c r="U23">
-        <v>1.004360163255154</v>
+        <v>1.00005751404153</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1872,61 +1872,61 @@
         <v>1.03</v>
       </c>
       <c r="C24">
-        <v>1.02142487479145</v>
+        <v>1.021341424696769</v>
       </c>
       <c r="D24">
-        <v>1.015724918319936</v>
+        <v>1.014968999367217</v>
       </c>
       <c r="E24">
-        <v>1.006308275074635</v>
+        <v>1.004521298774415</v>
       </c>
       <c r="F24">
-        <v>1.005815306826409</v>
+        <v>1.003991662369027</v>
       </c>
       <c r="G24">
-        <v>1.005477370806868</v>
+        <v>1.003620355569393</v>
       </c>
       <c r="H24">
-        <v>1.005091433209124</v>
+        <v>1.00323350625451</v>
       </c>
       <c r="I24">
-        <v>1.004828547601098</v>
+        <v>1.002929799982777</v>
       </c>
       <c r="J24">
-        <v>1.00487319060847</v>
+        <v>1.002974707750346</v>
       </c>
       <c r="K24">
-        <v>1.004609082206228</v>
+        <v>1.002702068417455</v>
       </c>
       <c r="L24">
-        <v>1.004278539684096</v>
+        <v>1.002351647656751</v>
       </c>
       <c r="M24">
-        <v>1.004228575036308</v>
+        <v>1.002293368527044</v>
       </c>
       <c r="N24">
-        <v>1.022061284486923</v>
+        <v>1.022045517917197</v>
       </c>
       <c r="O24">
-        <v>1.020639341486579</v>
+        <v>1.020217238135621</v>
       </c>
       <c r="P24">
-        <v>1.019818785046902</v>
+        <v>1.019396331383061</v>
       </c>
       <c r="Q24">
-        <v>1.004857318064029</v>
+        <v>1.002066907743038</v>
       </c>
       <c r="R24">
-        <v>1.020623219906804</v>
+        <v>1.01894306344149</v>
       </c>
       <c r="S24">
-        <v>1.005335607287259</v>
+        <v>1.00258415768755</v>
       </c>
       <c r="T24">
-        <v>1.00421271268135</v>
+        <v>1.001897462270677</v>
       </c>
       <c r="U24">
-        <v>1.006166602703792</v>
+        <v>1.003097008491306</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -1937,61 +1937,61 @@
         <v>1.03</v>
       </c>
       <c r="C25">
-        <v>1.021754289578721</v>
+        <v>1.021716720297421</v>
       </c>
       <c r="D25">
-        <v>1.016275206969454</v>
+        <v>1.015916554672156</v>
       </c>
       <c r="E25">
-        <v>1.007200778774723</v>
+        <v>1.006349250791169</v>
       </c>
       <c r="F25">
-        <v>1.006724865978073</v>
+        <v>1.005857678583578</v>
       </c>
       <c r="G25">
-        <v>1.006398628072935</v>
+        <v>1.005517196884526</v>
       </c>
       <c r="H25">
-        <v>1.006026518078672</v>
+        <v>1.005144666981509</v>
       </c>
       <c r="I25">
-        <v>1.005774971681789</v>
+        <v>1.004857136011943</v>
       </c>
       <c r="J25">
-        <v>1.005816673336593</v>
+        <v>1.004898962841325</v>
       </c>
       <c r="K25">
-        <v>1.005561456030448</v>
+        <v>1.004635534010041</v>
       </c>
       <c r="L25">
-        <v>1.005242268504495</v>
+        <v>1.004296899941357</v>
       </c>
       <c r="M25">
-        <v>1.005194089672786</v>
+        <v>1.004240486460042</v>
       </c>
       <c r="N25">
-        <v>1.022319763117535</v>
+        <v>1.022312534643092</v>
       </c>
       <c r="O25">
-        <v>1.020942606382199</v>
+        <v>1.020732887063272</v>
       </c>
       <c r="P25">
-        <v>1.020147695657128</v>
+        <v>1.019937807660049</v>
       </c>
       <c r="Q25">
-        <v>1.005800785889305</v>
+        <v>1.004504010563682</v>
       </c>
       <c r="R25">
-        <v>1.020926480012182</v>
+        <v>1.020092919670222</v>
       </c>
       <c r="S25">
-        <v>1.006256965600943</v>
+        <v>1.004995377985497</v>
       </c>
       <c r="T25">
-        <v>1.005178212059562</v>
+        <v>1.003845293492152</v>
       </c>
       <c r="U25">
-        <v>1.00705920411525</v>
+        <v>1.005700452727246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add change trafo size, peak_hour colormap plot, ev-per-cs setter, n_parallel_charged-getter
</commit_message>
<xml_diff>
--- a/PRO1/step_3/results/res_bus/vm_pu.xlsx
+++ b/PRO1/step_3/results/res_bus/vm_pu.xlsx
@@ -442,61 +442,61 @@
         <v>1.03</v>
       </c>
       <c r="C2">
-        <v>1.022260583353094</v>
+        <v>1.022285147001913</v>
       </c>
       <c r="D2">
-        <v>1.016940257313771</v>
+        <v>1.01718578158766</v>
       </c>
       <c r="E2">
-        <v>1.008114490211418</v>
+        <v>1.00869958488894</v>
       </c>
       <c r="F2">
-        <v>1.007655668441395</v>
+        <v>1.008251166439402</v>
       </c>
       <c r="G2">
-        <v>1.007338824045227</v>
+        <v>1.007943786846957</v>
       </c>
       <c r="H2">
-        <v>1.006988730819892</v>
+        <v>1.007593967990591</v>
       </c>
       <c r="I2">
-        <v>1.006720771515332</v>
+        <v>1.007360695766427</v>
       </c>
       <c r="J2">
-        <v>1.006757813590917</v>
+        <v>1.007397653642061</v>
       </c>
       <c r="K2">
-        <v>1.006514113243308</v>
+        <v>1.007156767555552</v>
       </c>
       <c r="L2">
-        <v>1.006206657536685</v>
+        <v>1.00685588291752</v>
       </c>
       <c r="M2">
-        <v>1.006158604565843</v>
+        <v>1.006810582744291</v>
       </c>
       <c r="N2">
-        <v>1.022730909631061</v>
+        <v>1.022734980948664</v>
       </c>
       <c r="O2">
-        <v>1.021304697376185</v>
+        <v>1.021430049851221</v>
       </c>
       <c r="P2">
-        <v>1.020551049093512</v>
+        <v>1.02067649724301</v>
       </c>
       <c r="Q2">
-        <v>1.006236606406304</v>
+        <v>1.007381741222288</v>
       </c>
       <c r="R2">
-        <v>1.020915632460395</v>
+        <v>1.021413915781757</v>
       </c>
       <c r="S2">
-        <v>1.006944760077447</v>
+        <v>1.00780229338222</v>
       </c>
       <c r="T2">
-        <v>1.006016915786869</v>
+        <v>1.006794679597638</v>
       </c>
       <c r="U2">
-        <v>1.007847062618489</v>
+        <v>1.008683651904422</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -507,61 +507,61 @@
         <v>1.03</v>
       </c>
       <c r="C3">
-        <v>1.022638495376116</v>
+        <v>1.022651444456785</v>
       </c>
       <c r="D3">
-        <v>1.01766432488076</v>
+        <v>1.017799317063514</v>
       </c>
       <c r="E3">
-        <v>1.009373809410904</v>
+        <v>1.009696498061694</v>
       </c>
       <c r="F3">
-        <v>1.0089393120861</v>
+        <v>1.009267200711153</v>
       </c>
       <c r="G3">
-        <v>1.008640318824184</v>
+        <v>1.00897293623579</v>
       </c>
       <c r="H3">
-        <v>1.008305856600393</v>
+        <v>1.008638619586681</v>
       </c>
       <c r="I3">
-        <v>1.008073363565869</v>
+        <v>1.008418049074436</v>
       </c>
       <c r="J3">
-        <v>1.00810706832818</v>
+        <v>1.008451709632978</v>
       </c>
       <c r="K3">
-        <v>1.007876057066866</v>
+        <v>1.008220790090022</v>
       </c>
       <c r="L3">
-        <v>1.007587781284021</v>
+        <v>1.007932633627258</v>
       </c>
       <c r="M3">
-        <v>1.007544463488786</v>
+        <v>1.007889335253258</v>
       </c>
       <c r="N3">
-        <v>1.023020853147901</v>
+        <v>1.023023459945867</v>
       </c>
       <c r="O3">
-        <v>1.021685534215698</v>
+        <v>1.021768915316444</v>
       </c>
       <c r="P3">
-        <v>1.020960772800367</v>
+        <v>1.021044215156406</v>
       </c>
       <c r="Q3">
-        <v>1.007839639001107</v>
+        <v>1.008435780563791</v>
       </c>
       <c r="R3">
-        <v>1.02142125391089</v>
+        <v>1.021752775894406</v>
       </c>
       <c r="S3">
-        <v>1.00837301488063</v>
+        <v>1.008831555007679</v>
       </c>
       <c r="T3">
-        <v>1.007528548753169</v>
+        <v>1.007873415067094</v>
       </c>
       <c r="U3">
-        <v>1.009106677710127</v>
+        <v>1.009680549330364</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -572,61 +572,61 @@
         <v>1.03</v>
       </c>
       <c r="C4">
-        <v>1.023012795258614</v>
+        <v>1.02303045990309</v>
       </c>
       <c r="D4">
-        <v>1.018269289579723</v>
+        <v>1.018457524839949</v>
       </c>
       <c r="E4">
-        <v>1.01033675842365</v>
+        <v>1.010787487974295</v>
       </c>
       <c r="F4">
-        <v>1.009926986977047</v>
+        <v>1.010382957997341</v>
       </c>
       <c r="G4">
-        <v>1.009646114445061</v>
+        <v>1.010106839196601</v>
       </c>
       <c r="H4">
-        <v>1.009327626104075</v>
+        <v>1.00978854502242</v>
       </c>
       <c r="I4">
-        <v>1.00907712174525</v>
+        <v>1.009571488758209</v>
       </c>
       <c r="J4">
-        <v>1.009107434743069</v>
+        <v>1.009601740039795</v>
       </c>
       <c r="K4">
-        <v>1.008881418796281</v>
+        <v>1.009381117378995</v>
       </c>
       <c r="L4">
-        <v>1.008593584247096</v>
+        <v>1.009106111242643</v>
       </c>
       <c r="M4">
-        <v>1.008546904162378</v>
+        <v>1.009064881192685</v>
       </c>
       <c r="N4">
-        <v>1.023319199768858</v>
+        <v>1.023320448473356</v>
       </c>
       <c r="O4">
-        <v>1.022076360174377</v>
+        <v>1.022117955738541</v>
       </c>
       <c r="P4">
-        <v>1.021381436758713</v>
+        <v>1.021423061652893</v>
       </c>
       <c r="Q4">
-        <v>1.008840240520714</v>
+        <v>1.009585792805222</v>
       </c>
       <c r="R4">
-        <v>1.021936385247691</v>
+        <v>1.022101810803212</v>
       </c>
       <c r="S4">
-        <v>1.009504806491458</v>
+        <v>1.010090883985653</v>
       </c>
       <c r="T4">
-        <v>1.008279578263803</v>
+        <v>1.009048942438102</v>
       </c>
       <c r="U4">
-        <v>1.010069852443143</v>
+        <v>1.010771522010158</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -637,61 +637,61 @@
         <v>1.03</v>
       </c>
       <c r="C5">
-        <v>1.02302480189348</v>
+        <v>1.02303234497713</v>
       </c>
       <c r="D5">
-        <v>1.018380055808593</v>
+        <v>1.018460687785302</v>
       </c>
       <c r="E5">
-        <v>1.010599498094862</v>
+        <v>1.010792633532488</v>
       </c>
       <c r="F5">
-        <v>1.010189957966755</v>
+        <v>1.01038820246331</v>
       </c>
       <c r="G5">
-        <v>1.009909244707296</v>
+        <v>1.010112151498275</v>
       </c>
       <c r="H5">
-        <v>1.0095909452662</v>
+        <v>1.009793937534582</v>
       </c>
       <c r="I5">
-        <v>1.009362074790257</v>
+        <v>1.009576947010709</v>
       </c>
       <c r="J5">
-        <v>1.009392335827987</v>
+        <v>1.009607181232212</v>
       </c>
       <c r="K5">
-        <v>1.009169079805256</v>
+        <v>1.009386610135808</v>
       </c>
       <c r="L5">
-        <v>1.008887744295604</v>
+        <v>1.00911166985086</v>
       </c>
       <c r="M5">
-        <v>1.008843804828139</v>
+        <v>1.009070450157624</v>
       </c>
       <c r="N5">
-        <v>1.023318071368558</v>
+        <v>1.023321936726942</v>
       </c>
       <c r="O5">
-        <v>1.021994655427625</v>
+        <v>1.022119705290602</v>
       </c>
       <c r="P5">
-        <v>1.021299822802728</v>
+        <v>1.021424960830191</v>
       </c>
       <c r="Q5">
-        <v>1.00925100026342</v>
+        <v>1.009591233911692</v>
       </c>
       <c r="R5">
-        <v>1.021605833732119</v>
+        <v>1.022103560327637</v>
       </c>
       <c r="S5">
-        <v>1.009767965362207</v>
+        <v>1.010096196201463</v>
       </c>
       <c r="T5">
-        <v>1.008702409532029</v>
+        <v>1.009054511315077</v>
       </c>
       <c r="U5">
-        <v>1.010583535101881</v>
+        <v>1.010776667487074</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -702,61 +702,61 @@
         <v>1.03</v>
       </c>
       <c r="C6">
-        <v>1.023255897408271</v>
+        <v>1.023273096800444</v>
       </c>
       <c r="D6">
-        <v>1.018677470037257</v>
+        <v>1.018864800887998</v>
       </c>
       <c r="E6">
-        <v>1.01100097937691</v>
+        <v>1.011450228362985</v>
       </c>
       <c r="F6">
-        <v>1.010598945241475</v>
+        <v>1.011058443968306</v>
       </c>
       <c r="G6">
-        <v>1.010322220216712</v>
+        <v>1.010791066721083</v>
       </c>
       <c r="H6">
-        <v>1.010014069526862</v>
+        <v>1.010483108715766</v>
       </c>
       <c r="I6">
-        <v>1.009792430196759</v>
+        <v>1.010274522940922</v>
       </c>
       <c r="J6">
-        <v>1.009820542210462</v>
+        <v>1.010302575830803</v>
       </c>
       <c r="K6">
-        <v>1.009603815441855</v>
+        <v>1.010088597794496</v>
       </c>
       <c r="L6">
-        <v>1.009330817851442</v>
+        <v>1.009822077289054</v>
       </c>
       <c r="M6">
-        <v>1.009288189964943</v>
+        <v>1.00978218181126</v>
       </c>
       <c r="N6">
-        <v>1.023512101776491</v>
+        <v>1.023510875509177</v>
       </c>
       <c r="O6">
-        <v>1.022343296695319</v>
+        <v>1.022301734050026</v>
       </c>
       <c r="P6">
-        <v>1.021667692891168</v>
+        <v>1.021626101731756</v>
       </c>
       <c r="Q6">
-        <v>1.009553515284103</v>
+        <v>1.01028661752613</v>
       </c>
       <c r="R6">
-        <v>1.02232714820717</v>
+        <v>1.022161782947423</v>
       </c>
       <c r="S6">
-        <v>1.010055310832054</v>
+        <v>1.010775100700417</v>
       </c>
       <c r="T6">
-        <v>1.009146843064988</v>
+        <v>1.009766231726507</v>
       </c>
       <c r="U6">
-        <v>1.010734228824527</v>
+        <v>1.011434251930486</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -767,61 +767,61 @@
         <v>1.03</v>
       </c>
       <c r="C7">
-        <v>1.023049280008193</v>
+        <v>1.023082861981823</v>
       </c>
       <c r="D7">
-        <v>1.018171546571496</v>
+        <v>1.018522879991381</v>
       </c>
       <c r="E7">
-        <v>1.01003305254734</v>
+        <v>1.010873233699438</v>
       </c>
       <c r="F7">
-        <v>1.009610826140785</v>
+        <v>1.010471547589995</v>
       </c>
       <c r="G7">
-        <v>1.009317920872699</v>
+        <v>1.010197379171471</v>
       </c>
       <c r="H7">
-        <v>1.009001563644202</v>
+        <v>1.009881390676519</v>
       </c>
       <c r="I7">
-        <v>1.008749454436298</v>
+        <v>1.009666221449531</v>
       </c>
       <c r="J7">
-        <v>1.008779331609329</v>
+        <v>1.009695984590893</v>
       </c>
       <c r="K7">
-        <v>1.008554690496652</v>
+        <v>1.009476845125709</v>
       </c>
       <c r="L7">
-        <v>1.008268606702818</v>
+        <v>1.009203732727853</v>
       </c>
       <c r="M7">
-        <v>1.008222199928343</v>
+        <v>1.009162800392238</v>
       </c>
       <c r="N7">
-        <v>1.02336119203823</v>
+        <v>1.023363719215658</v>
       </c>
       <c r="O7">
-        <v>1.022085561449552</v>
+        <v>1.022168825642667</v>
       </c>
       <c r="P7">
-        <v>1.02139496045465</v>
+        <v>1.021478283003365</v>
       </c>
       <c r="Q7">
-        <v>1.008132043769834</v>
+        <v>1.009680035867673</v>
       </c>
       <c r="R7">
-        <v>1.021821372549789</v>
+        <v>1.022152679903884</v>
       </c>
       <c r="S7">
-        <v>1.008797971285038</v>
+        <v>1.010181422528439</v>
       </c>
       <c r="T7">
-        <v>1.007954797676398</v>
+        <v>1.009146860090967</v>
       </c>
       <c r="U7">
-        <v>1.009639964370616</v>
+        <v>1.010732059023049</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -832,61 +832,61 @@
         <v>1.03</v>
       </c>
       <c r="C8">
-        <v>1.022599087587895</v>
+        <v>1.022628219223735</v>
       </c>
       <c r="D8">
-        <v>1.017462031105671</v>
+        <v>1.017760394738771</v>
       </c>
       <c r="E8">
-        <v>1.008920937441804</v>
+        <v>1.009633231514454</v>
       </c>
       <c r="F8">
-        <v>1.008479974281017</v>
+        <v>1.009202719842634</v>
       </c>
       <c r="G8">
-        <v>1.008175380509967</v>
+        <v>1.008907622464649</v>
       </c>
       <c r="H8">
-        <v>1.007839758045094</v>
+        <v>1.00857232132004</v>
       </c>
       <c r="I8">
-        <v>1.007594465417679</v>
+        <v>1.008350944295946</v>
       </c>
       <c r="J8">
-        <v>1.007628432572822</v>
+        <v>1.008384814253474</v>
       </c>
       <c r="K8">
-        <v>1.007394043328788</v>
+        <v>1.008153261783636</v>
       </c>
       <c r="L8">
-        <v>1.007098480669374</v>
+        <v>1.00786429701981</v>
       </c>
       <c r="M8">
-        <v>1.007052299449739</v>
+        <v>1.007820871521551</v>
       </c>
       <c r="N8">
-        <v>1.02300117972796</v>
+        <v>1.023005156338313</v>
       </c>
       <c r="O8">
-        <v>1.021622196403153</v>
+        <v>1.021747409679759</v>
       </c>
       <c r="P8">
-        <v>1.020895570470776</v>
+        <v>1.021020875965341</v>
       </c>
       <c r="Q8">
-        <v>1.007234473764515</v>
+        <v>1.008368886240937</v>
       </c>
       <c r="R8">
-        <v>1.021233243453742</v>
+        <v>1.021731270597415</v>
       </c>
       <c r="S8">
-        <v>1.007781620116075</v>
+        <v>1.008766234123949</v>
       </c>
       <c r="T8">
-        <v>1.006910708549217</v>
+        <v>1.007804952416811</v>
       </c>
       <c r="U8">
-        <v>1.008273737375279</v>
+        <v>1.009617283783582</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -897,61 +897,61 @@
         <v>1.03</v>
       </c>
       <c r="C9">
-        <v>1.02132709904349</v>
+        <v>1.021363486022933</v>
       </c>
       <c r="D9">
-        <v>1.015310493493901</v>
+        <v>1.015645085283198</v>
       </c>
       <c r="E9">
-        <v>1.005407346242882</v>
+        <v>1.006199523560017</v>
       </c>
       <c r="F9">
-        <v>1.004910623174902</v>
+        <v>1.005703277769442</v>
       </c>
       <c r="G9">
-        <v>1.004570110067247</v>
+        <v>1.005363093886676</v>
       </c>
       <c r="H9">
-        <v>1.004181124467152</v>
+        <v>1.004974499376951</v>
       </c>
       <c r="I9">
-        <v>1.003807358148684</v>
+        <v>1.004709436670169</v>
       </c>
       <c r="J9">
-        <v>1.003852690263196</v>
+        <v>1.004754642571241</v>
       </c>
       <c r="K9">
-        <v>1.003567965425974</v>
+        <v>1.004488824761512</v>
       </c>
       <c r="L9">
-        <v>1.003190088728251</v>
+        <v>1.004156099521488</v>
       </c>
       <c r="M9">
-        <v>1.003120542595835</v>
+        <v>1.004105791718521</v>
       </c>
       <c r="N9">
-        <v>1.02200195855004</v>
+        <v>1.022010969472217</v>
       </c>
       <c r="O9">
-        <v>1.020328076609923</v>
+        <v>1.020580323946096</v>
       </c>
       <c r="P9">
-        <v>1.019502326328291</v>
+        <v>1.019754784223464</v>
       </c>
       <c r="Q9">
-        <v>1.003457355467199</v>
+        <v>1.004738771899334</v>
       </c>
       <c r="R9">
-        <v>1.019561879469991</v>
+        <v>1.020564203298537</v>
       </c>
       <c r="S9">
-        <v>1.004428246822216</v>
+        <v>1.00522131781511</v>
       </c>
       <c r="T9">
-        <v>1.002212872875783</v>
+        <v>1.004089931295582</v>
       </c>
       <c r="U9">
-        <v>1.005139279870237</v>
+        <v>1.006183630065392</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -962,61 +962,61 @@
         <v>1.03</v>
       </c>
       <c r="C10">
-        <v>1.016711825345493</v>
+        <v>1.016814234525497</v>
       </c>
       <c r="D10">
-        <v>1.007376494128347</v>
+        <v>1.008122392769343</v>
       </c>
       <c r="E10">
-        <v>0.9923528122019485</v>
+        <v>0.9940787794780779</v>
       </c>
       <c r="F10">
-        <v>0.9915935287109746</v>
+        <v>0.9933569635440676</v>
       </c>
       <c r="G10">
-        <v>0.9910658154278791</v>
+        <v>0.9928632470425371</v>
       </c>
       <c r="H10">
-        <v>0.9904889697845853</v>
+        <v>0.9922876376532933</v>
       </c>
       <c r="I10">
-        <v>0.9900404704033</v>
+        <v>0.9918590550176537</v>
       </c>
       <c r="J10">
-        <v>0.9901257933637626</v>
+        <v>0.9919440492234762</v>
       </c>
       <c r="K10">
-        <v>0.9897254125419274</v>
+        <v>0.9915579309088464</v>
       </c>
       <c r="L10">
-        <v>0.9892056279367476</v>
+        <v>0.9910715578341366</v>
       </c>
       <c r="M10">
-        <v>0.989117124393659</v>
+        <v>0.9909970864997705</v>
       </c>
       <c r="N10">
-        <v>1.018464376418338</v>
+        <v>1.018471851288541</v>
       </c>
       <c r="O10">
-        <v>1.016270970584856</v>
+        <v>1.016441188574724</v>
       </c>
       <c r="P10">
-        <v>1.015101643210832</v>
+        <v>1.015272061620074</v>
       </c>
       <c r="Q10">
-        <v>0.9897253625033329</v>
+        <v>0.9919283809021879</v>
       </c>
       <c r="R10">
-        <v>1.015754402882731</v>
+        <v>1.016425133307166</v>
       </c>
       <c r="S10">
-        <v>0.9901472400161411</v>
+        <v>0.9928475642019957</v>
       </c>
       <c r="T10">
-        <v>0.988457390970684</v>
+        <v>0.9909814331362977</v>
       </c>
       <c r="U10">
-        <v>0.9910426106927058</v>
+        <v>0.994063077437509</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1027,61 +1027,61 @@
         <v>1.03</v>
       </c>
       <c r="C11">
-        <v>1.012482774666418</v>
+        <v>1.012579261596185</v>
       </c>
       <c r="D11">
-        <v>1.000527819163288</v>
+        <v>1.001129543381241</v>
       </c>
       <c r="E11">
-        <v>0.9814713527145551</v>
+        <v>0.9828381145814301</v>
       </c>
       <c r="F11">
-        <v>0.9805046965670281</v>
+        <v>0.981904212223619</v>
       </c>
       <c r="G11">
-        <v>0.9798346910784728</v>
+        <v>0.9812638691735526</v>
       </c>
       <c r="H11">
-        <v>0.9790900177944137</v>
+        <v>0.9805204341534941</v>
       </c>
       <c r="I11">
-        <v>0.9784914334243489</v>
+        <v>0.9799631021533421</v>
       </c>
       <c r="J11">
-        <v>0.9786124715381187</v>
+        <v>0.9800838190275935</v>
       </c>
       <c r="K11">
-        <v>0.9781066200043835</v>
+        <v>0.9795896827800931</v>
       </c>
       <c r="L11">
-        <v>0.9774550138803533</v>
+        <v>0.9789653319238952</v>
       </c>
       <c r="M11">
-        <v>0.9773474582336817</v>
+        <v>0.978869162257457</v>
       </c>
       <c r="N11">
-        <v>1.015214092536266</v>
+        <v>1.015240276294989</v>
       </c>
       <c r="O11">
-        <v>1.012203458501552</v>
+        <v>1.012681064882455</v>
       </c>
       <c r="P11">
-        <v>1.010730957037989</v>
+        <v>1.011209271566259</v>
       </c>
       <c r="Q11">
-        <v>0.9779458737311366</v>
+        <v>0.9800683380453971</v>
       </c>
       <c r="R11">
-        <v>1.010790107388613</v>
+        <v>1.012665069008192</v>
       </c>
       <c r="S11">
-        <v>0.9789057009631953</v>
+        <v>0.9811193715294363</v>
       </c>
       <c r="T11">
-        <v>0.9768113065354642</v>
+        <v>0.9788537004614561</v>
       </c>
       <c r="U11">
-        <v>0.9808066383507729</v>
+        <v>0.9826937993875019</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1092,61 +1092,61 @@
         <v>1.03</v>
       </c>
       <c r="C12">
-        <v>1.005009013791476</v>
+        <v>1.005270789924841</v>
       </c>
       <c r="D12">
-        <v>0.987899540216739</v>
+        <v>0.9892122949438726</v>
       </c>
       <c r="E12">
-        <v>0.9609671724810916</v>
+        <v>0.9638550446444304</v>
       </c>
       <c r="F12">
-        <v>0.9596484323175846</v>
+        <v>0.9625619972372293</v>
       </c>
       <c r="G12">
-        <v>0.9587356046986832</v>
+        <v>0.9616717244623377</v>
       </c>
       <c r="H12">
-        <v>0.9577103911307245</v>
+        <v>0.9606499612668414</v>
       </c>
       <c r="I12">
-        <v>0.9567374605263895</v>
+        <v>0.959880749307347</v>
       </c>
       <c r="J12">
-        <v>0.9569183358487727</v>
+        <v>0.9600607346844061</v>
       </c>
       <c r="K12">
-        <v>0.956222927563005</v>
+        <v>0.9593845271472139</v>
       </c>
       <c r="L12">
-        <v>0.9553193525351332</v>
+        <v>0.9585244489847523</v>
       </c>
       <c r="M12">
-        <v>0.9551665179820705</v>
+        <v>0.9583894080726866</v>
       </c>
       <c r="N12">
-        <v>1.009747227326449</v>
+        <v>1.009783371471103</v>
       </c>
       <c r="O12">
-        <v>1.005835892228512</v>
+        <v>1.006368473770558</v>
       </c>
       <c r="P12">
-        <v>1.003873037441537</v>
+        <v>1.004406674851278</v>
       </c>
       <c r="Q12">
-        <v>0.9548692627713272</v>
+        <v>0.9600455699782323</v>
       </c>
       <c r="R12">
-        <v>1.004283176480023</v>
+        <v>1.006352577607267</v>
       </c>
       <c r="S12">
-        <v>0.9576510331788527</v>
+        <v>0.9611272144318036</v>
       </c>
       <c r="T12">
-        <v>0.9542137472449568</v>
+        <v>0.9582421821020901</v>
       </c>
       <c r="U12">
-        <v>0.9593404722985189</v>
+        <v>0.9638398200049691</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1157,61 +1157,61 @@
         <v>1.03</v>
       </c>
       <c r="C13">
-        <v>0.9987377913338281</v>
+        <v>0.9991679966197937</v>
       </c>
       <c r="D13">
-        <v>0.9775327710641171</v>
+        <v>0.979431634999295</v>
       </c>
       <c r="E13">
-        <v>0.9443785680777389</v>
+        <v>0.9484622593957603</v>
       </c>
       <c r="F13">
-        <v>0.942735700859437</v>
+        <v>0.9468983952154666</v>
       </c>
       <c r="G13">
-        <v>0.941590340051615</v>
+        <v>0.945823617863402</v>
       </c>
       <c r="H13">
-        <v>0.940338759443089</v>
+        <v>0.9445781079160566</v>
       </c>
       <c r="I13">
-        <v>0.9392092997053345</v>
+        <v>0.9436004224575046</v>
       </c>
       <c r="J13">
-        <v>0.9394384405444979</v>
+        <v>0.9438280814380111</v>
       </c>
       <c r="K13">
-        <v>0.9385703882955626</v>
+        <v>0.9430103344577621</v>
       </c>
       <c r="L13">
-        <v>0.9374163171939207</v>
+        <v>0.9419725211111718</v>
       </c>
       <c r="M13">
-        <v>0.9372068283607066</v>
+        <v>0.941811338369978</v>
       </c>
       <c r="N13">
-        <v>1.005274161381137</v>
+        <v>1.005317269659471</v>
       </c>
       <c r="O13">
-        <v>1.000606799797854</v>
+        <v>1.001150612926383</v>
       </c>
       <c r="P13">
-        <v>0.9982603675028539</v>
+        <v>0.9988054745375345</v>
       </c>
       <c r="Q13">
-        <v>0.9380535656506952</v>
+        <v>0.9435444178233119</v>
       </c>
       <c r="R13">
-        <v>0.9987824965162884</v>
+        <v>1.000881534605665</v>
       </c>
       <c r="S13">
-        <v>0.9393646996381034</v>
+        <v>0.9454056715128591</v>
       </c>
       <c r="T13">
-        <v>0.9349703149021142</v>
+        <v>0.9417964619234142</v>
       </c>
       <c r="U13">
-        <v>0.9427226076182712</v>
+        <v>0.9484472778941104</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1222,61 +1222,61 @@
         <v>1.03</v>
       </c>
       <c r="C14">
-        <v>0.9981327963057236</v>
+        <v>0.9986046686511212</v>
       </c>
       <c r="D14">
-        <v>0.9765162210460857</v>
+        <v>0.9785818487264724</v>
       </c>
       <c r="E14">
-        <v>0.9427395580076526</v>
+        <v>0.9471744317449415</v>
       </c>
       <c r="F14">
-        <v>0.9410702970427287</v>
+        <v>0.9455958948862359</v>
       </c>
       <c r="G14">
-        <v>0.9399068075166912</v>
+        <v>0.9445135280564046</v>
       </c>
       <c r="H14">
-        <v>0.9386339531105692</v>
+        <v>0.9432473928108169</v>
       </c>
       <c r="I14">
-        <v>0.9374748291118029</v>
+        <v>0.9422315737003187</v>
       </c>
       <c r="J14">
-        <v>0.9377085141931842</v>
+        <v>0.9424636290050548</v>
       </c>
       <c r="K14">
-        <v>0.936832521944934</v>
+        <v>0.9416297166770886</v>
       </c>
       <c r="L14">
-        <v>0.9356748121285342</v>
+        <v>0.9405680661886365</v>
       </c>
       <c r="M14">
-        <v>0.9354685128988517</v>
+        <v>0.9404012977539142</v>
       </c>
       <c r="N14">
-        <v>1.004873754376655</v>
+        <v>1.004901796579473</v>
       </c>
       <c r="O14">
-        <v>1.000354169855862</v>
+        <v>1.000714956550834</v>
       </c>
       <c r="P14">
-        <v>0.9979730180529768</v>
+        <v>0.9983346761872731</v>
       </c>
       <c r="Q14">
-        <v>0.9358994308534326</v>
+        <v>0.9423144144727951</v>
       </c>
       <c r="R14">
-        <v>0.9991847761858649</v>
+        <v>1.000572667243163</v>
       </c>
       <c r="S14">
-        <v>0.9376770042739817</v>
+        <v>0.9443645737489411</v>
       </c>
       <c r="T14">
-        <v>0.9335130398442163</v>
+        <v>0.9402518201331235</v>
       </c>
       <c r="U14">
-        <v>0.9409404215658662</v>
+        <v>0.947159470585263</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1287,61 +1287,61 @@
         <v>1.03</v>
       </c>
       <c r="C15">
-        <v>0.9986579036317065</v>
+        <v>0.9990691112048488</v>
       </c>
       <c r="D15">
-        <v>0.9774808178050718</v>
+        <v>0.979298664546455</v>
       </c>
       <c r="E15">
-        <v>0.9443660965707368</v>
+        <v>0.9482764669429721</v>
       </c>
       <c r="F15">
-        <v>0.9427411728142285</v>
+        <v>0.9467187628932123</v>
       </c>
       <c r="G15">
-        <v>0.9416132114507911</v>
+        <v>0.9456506791649187</v>
       </c>
       <c r="H15">
-        <v>0.9403581632159033</v>
+        <v>0.9444014367413697</v>
       </c>
       <c r="I15">
-        <v>0.9391834551914862</v>
+        <v>0.9434113385908947</v>
       </c>
       <c r="J15">
-        <v>0.9394133395958276</v>
+        <v>0.9436397926515715</v>
       </c>
       <c r="K15">
-        <v>0.938548887507062</v>
+        <v>0.9428167966706984</v>
       </c>
       <c r="L15">
-        <v>0.9374060149564929</v>
+        <v>0.941769099804964</v>
       </c>
       <c r="M15">
-        <v>0.9372020991826759</v>
+        <v>0.941604527438661</v>
       </c>
       <c r="N15">
-        <v>1.005192369983939</v>
+        <v>1.005236113519161</v>
       </c>
       <c r="O15">
-        <v>1.000471428706037</v>
+        <v>1.001016555066448</v>
       </c>
       <c r="P15">
-        <v>0.9981183256356716</v>
+        <v>0.9986647528673597</v>
       </c>
       <c r="Q15">
-        <v>0.9377484056140301</v>
+        <v>0.9436248873265533</v>
       </c>
       <c r="R15">
-        <v>0.998514562355555</v>
+        <v>1.000620179481709</v>
       </c>
       <c r="S15">
-        <v>0.9399522658920987</v>
+        <v>0.9455018686515984</v>
       </c>
       <c r="T15">
-        <v>0.9352503723074369</v>
+        <v>0.941455203467457</v>
       </c>
       <c r="U15">
-        <v>0.9425701515771796</v>
+        <v>0.9479940029316447</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1352,61 +1352,61 @@
         <v>1.03</v>
       </c>
       <c r="C16">
-        <v>0.998699398978526</v>
+        <v>0.9990990217988024</v>
       </c>
       <c r="D16">
-        <v>0.9776218012631885</v>
+        <v>0.9793946597972771</v>
       </c>
       <c r="E16">
-        <v>0.9446550720291981</v>
+        <v>0.9484711443899461</v>
       </c>
       <c r="F16">
-        <v>0.943025697772744</v>
+        <v>0.9469143515071947</v>
       </c>
       <c r="G16">
-        <v>0.9418934203814534</v>
+        <v>0.9458468928185623</v>
       </c>
       <c r="H16">
-        <v>0.9406392372248302</v>
+        <v>0.944598389969418</v>
       </c>
       <c r="I16">
-        <v>0.9395230255972066</v>
+        <v>0.9436089209881274</v>
       </c>
       <c r="J16">
-        <v>0.9397526980363057</v>
+        <v>0.9438372122168404</v>
       </c>
       <c r="K16">
-        <v>0.9388859328028106</v>
+        <v>0.9430146921242556</v>
       </c>
       <c r="L16">
-        <v>0.937736829174897</v>
+        <v>0.9419676050562454</v>
       </c>
       <c r="M16">
-        <v>0.9375300405094651</v>
+        <v>0.9418031292276379</v>
       </c>
       <c r="N16">
-        <v>1.005194716189954</v>
+        <v>1.005253026490274</v>
       </c>
       <c r="O16">
-        <v>1.00039099613441</v>
+        <v>1.001117812489742</v>
       </c>
       <c r="P16">
-        <v>0.998038536618166</v>
+        <v>0.9987670867751097</v>
       </c>
       <c r="Q16">
-        <v>0.9387844001875572</v>
+        <v>0.943822303770445</v>
       </c>
       <c r="R16">
-        <v>0.998168071271893</v>
+        <v>1.000975567881905</v>
       </c>
       <c r="S16">
-        <v>0.9400926190221198</v>
+        <v>0.945698107078547</v>
       </c>
       <c r="T16">
-        <v>0.9354369309870125</v>
+        <v>0.9416538305754691</v>
       </c>
       <c r="U16">
-        <v>0.9428596928011719</v>
+        <v>0.9484561627500085</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1417,61 +1417,61 @@
         <v>1.03</v>
       </c>
       <c r="C17">
-        <v>0.9986046581550297</v>
+        <v>0.999136841114627</v>
       </c>
       <c r="D17">
-        <v>0.9770465374760666</v>
+        <v>0.9793825595764196</v>
       </c>
       <c r="E17">
-        <v>0.9433678261988624</v>
+        <v>0.9483859449904951</v>
       </c>
       <c r="F17">
-        <v>0.9417217808842819</v>
+        <v>0.9468206652184485</v>
       </c>
       <c r="G17">
-        <v>0.9405742184638808</v>
+        <v>0.9457449171299841</v>
       </c>
       <c r="H17">
-        <v>0.9393201323701914</v>
+        <v>0.944498260079398</v>
       </c>
       <c r="I17">
-        <v>0.9381650885239089</v>
+        <v>0.9435426901048459</v>
       </c>
       <c r="J17">
-        <v>0.9383948019027646</v>
+        <v>0.9437705856444407</v>
       </c>
       <c r="K17">
-        <v>0.9375368202469755</v>
+        <v>0.9429521193889016</v>
       </c>
       <c r="L17">
-        <v>0.9364087334870905</v>
+        <v>0.9419133870583388</v>
       </c>
       <c r="M17">
-        <v>0.9362109109019984</v>
+        <v>0.9417520598761547</v>
       </c>
       <c r="N17">
-        <v>1.005243227461577</v>
+        <v>1.005297486013601</v>
       </c>
       <c r="O17">
-        <v>1.000488264479699</v>
+        <v>1.001168817478008</v>
       </c>
       <c r="P17">
-        <v>0.9981396651739445</v>
+        <v>0.9988218388827838</v>
       </c>
       <c r="Q17">
-        <v>0.9361612460822412</v>
+        <v>0.9437556782504501</v>
       </c>
       <c r="R17">
-        <v>0.9983987072504698</v>
+        <v>1.001026578525464</v>
       </c>
       <c r="S17">
-        <v>0.9383460674545707</v>
+        <v>0.9453269381237015</v>
       </c>
       <c r="T17">
-        <v>0.9345401350771381</v>
+        <v>0.9417371843662482</v>
       </c>
       <c r="U17">
-        <v>0.9404309536729525</v>
+        <v>0.9481035103465146</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1482,61 +1482,61 @@
         <v>1.03</v>
       </c>
       <c r="C18">
-        <v>1.004534830888391</v>
+        <v>1.004996666910926</v>
       </c>
       <c r="D18">
-        <v>0.9864983978384183</v>
+        <v>0.9887478331778264</v>
       </c>
       <c r="E18">
-        <v>0.9581752280523791</v>
+        <v>0.963100394624579</v>
       </c>
       <c r="F18">
-        <v>0.95680276415192</v>
+        <v>0.961800226376054</v>
       </c>
       <c r="G18">
-        <v>0.9558443296536079</v>
+        <v>0.9609062886662625</v>
       </c>
       <c r="H18">
-        <v>0.9548064783740231</v>
+        <v>0.9598744566290048</v>
       </c>
       <c r="I18">
-        <v>0.953742339076379</v>
+        <v>0.9590980536539537</v>
       </c>
       <c r="J18">
-        <v>0.9539260029299139</v>
+        <v>0.9592801853580394</v>
       </c>
       <c r="K18">
-        <v>0.9532023262203336</v>
+        <v>0.9586002669842554</v>
       </c>
       <c r="L18">
-        <v>0.9522400626066423</v>
+        <v>0.9577385681054665</v>
       </c>
       <c r="M18">
-        <v>0.9520649612006401</v>
+        <v>0.9576050759620441</v>
       </c>
       <c r="N18">
-        <v>1.009531890073061</v>
+        <v>1.009585311052823</v>
       </c>
       <c r="O18">
-        <v>1.005381077023319</v>
+        <v>1.006140152316455</v>
       </c>
       <c r="P18">
-        <v>1.003400430273486</v>
+        <v>1.004161024335808</v>
       </c>
       <c r="Q18">
-        <v>0.9510236977069273</v>
+        <v>0.9592650329810867</v>
       </c>
       <c r="R18">
-        <v>1.003169620307694</v>
+        <v>1.006124259759632</v>
       </c>
       <c r="S18">
-        <v>0.9537928678409018</v>
+        <v>0.9604944969778623</v>
       </c>
       <c r="T18">
-        <v>0.9501447475846725</v>
+        <v>0.9575899500443986</v>
       </c>
       <c r="U18">
-        <v>0.9557099211639819</v>
+        <v>0.9626894813223259</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1547,61 +1547,61 @@
         <v>1.03</v>
       </c>
       <c r="C19">
-        <v>1.014240456569193</v>
+        <v>1.014631993067221</v>
       </c>
       <c r="D19">
-        <v>1.001985347122213</v>
+        <v>1.004395882194901</v>
       </c>
       <c r="E19">
-        <v>0.9825060917573073</v>
+        <v>0.9879745040824554</v>
       </c>
       <c r="F19">
-        <v>0.981566854047879</v>
+        <v>0.9871408362181683</v>
       </c>
       <c r="G19">
-        <v>0.9808997587228475</v>
+        <v>0.9865692324945922</v>
       </c>
       <c r="H19">
-        <v>0.9802331548905583</v>
+        <v>0.9859070657021238</v>
       </c>
       <c r="I19">
-        <v>0.9794672011534585</v>
+        <v>0.9854058989132322</v>
       </c>
       <c r="J19">
-        <v>0.9795718235400499</v>
+        <v>0.9855093292498712</v>
       </c>
       <c r="K19">
-        <v>0.97906027846354</v>
+        <v>0.9850675102888944</v>
       </c>
       <c r="L19">
-        <v>0.978338473977665</v>
+        <v>0.9845099871279789</v>
       </c>
       <c r="M19">
-        <v>0.9781835235768156</v>
+        <v>0.9844243259524126</v>
       </c>
       <c r="N19">
-        <v>1.016777103090166</v>
+        <v>1.016814662975463</v>
       </c>
       <c r="O19">
-        <v>1.013774849831582</v>
+        <v>1.014470401983127</v>
       </c>
       <c r="P19">
-        <v>1.012448467811389</v>
+        <v>1.013144948709212</v>
       </c>
       <c r="Q19">
-        <v>0.9772996810423099</v>
+        <v>0.985365322118458</v>
       </c>
       <c r="R19">
-        <v>1.011582407504162</v>
+        <v>1.014329615859043</v>
       </c>
       <c r="S19">
-        <v>0.9782198958966697</v>
+        <v>0.9864253470701912</v>
       </c>
       <c r="T19">
-        <v>0.974939899077974</v>
+        <v>0.9844087764094366</v>
       </c>
       <c r="U19">
-        <v>0.9798308483556265</v>
+        <v>0.9874438603245242</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1612,61 +1612,61 @@
         <v>1.03</v>
       </c>
       <c r="C20">
-        <v>1.016720706440919</v>
+        <v>1.016993975185224</v>
       </c>
       <c r="D20">
-        <v>1.006360345583179</v>
+        <v>1.008211905452195</v>
       </c>
       <c r="E20">
-        <v>0.9897826708085163</v>
+        <v>0.9940333645651582</v>
       </c>
       <c r="F20">
-        <v>0.9889947467453553</v>
+        <v>0.9933063813733618</v>
       </c>
       <c r="G20">
-        <v>0.988438925420245</v>
+        <v>0.9928055834822076</v>
       </c>
       <c r="H20">
-        <v>0.9878685713435873</v>
+        <v>0.9922382036366644</v>
       </c>
       <c r="I20">
-        <v>0.987226532372573</v>
+        <v>0.9918130432827641</v>
       </c>
       <c r="J20">
-        <v>0.9873106211155417</v>
+        <v>0.9918963091956718</v>
       </c>
       <c r="K20">
-        <v>0.98687850476116</v>
+        <v>0.9915128135876136</v>
       </c>
       <c r="L20">
-        <v>0.986277782582953</v>
+        <v>0.9910267678671212</v>
       </c>
       <c r="M20">
-        <v>0.9861532090487753</v>
+        <v>0.9909506023243406</v>
       </c>
       <c r="N20">
-        <v>1.018591224771914</v>
+        <v>1.018633813574398</v>
       </c>
       <c r="O20">
-        <v>1.015725099460699</v>
+        <v>1.016549455756345</v>
       </c>
       <c r="P20">
-        <v>1.014570697464714</v>
+        <v>1.015396012111086</v>
       </c>
       <c r="Q20">
-        <v>0.9854610556436039</v>
+        <v>0.9916249985896779</v>
       </c>
       <c r="R20">
-        <v>1.013009250367594</v>
+        <v>1.016283994988764</v>
       </c>
       <c r="S20">
-        <v>0.986591532053674</v>
+        <v>0.9924061591949507</v>
       </c>
       <c r="T20">
-        <v>0.98376114866292</v>
+        <v>0.990807216847349</v>
       </c>
       <c r="U20">
-        <v>0.9867174371258072</v>
+        <v>0.9936343995357819</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1677,61 +1677,61 @@
         <v>1.03</v>
       </c>
       <c r="C21">
-        <v>1.019214948684147</v>
+        <v>1.019480750293981</v>
       </c>
       <c r="D21">
-        <v>1.010424987172349</v>
+        <v>1.012419505188322</v>
       </c>
       <c r="E21">
-        <v>0.996265216698521</v>
+        <v>1.000897076100353</v>
       </c>
       <c r="F21">
-        <v>0.9956130252535789</v>
+        <v>1.00030482731351</v>
       </c>
       <c r="G21">
-        <v>0.9951528015592596</v>
+        <v>0.999898796933354</v>
       </c>
       <c r="H21">
-        <v>0.9946836398307588</v>
+        <v>0.9994323664950373</v>
       </c>
       <c r="I21">
-        <v>0.9940279738799883</v>
+        <v>0.9990817246871758</v>
       </c>
       <c r="J21">
-        <v>0.9940905456063903</v>
+        <v>0.99914350182752</v>
       </c>
       <c r="K21">
-        <v>0.993723892918601</v>
+        <v>0.9988249638212937</v>
       </c>
       <c r="L21">
-        <v>0.9932071875801385</v>
+        <v>0.9984219084762803</v>
       </c>
       <c r="M21">
-        <v>0.9930960579878894</v>
+        <v>0.9983588078465327</v>
       </c>
       <c r="N21">
-        <v>1.020498826812595</v>
+        <v>1.020548749580749</v>
       </c>
       <c r="O21">
-        <v>1.017790533949064</v>
+        <v>1.018827125290082</v>
       </c>
       <c r="P21">
-        <v>1.016820507367092</v>
+        <v>1.01785811274824</v>
       </c>
       <c r="Q21">
-        <v>0.9913123303757265</v>
+        <v>0.9990010377626097</v>
       </c>
       <c r="R21">
-        <v>1.014547517001705</v>
+        <v>1.018686805532224</v>
       </c>
       <c r="S21">
-        <v>0.9935831161598898</v>
+        <v>0.9997564169413224</v>
       </c>
       <c r="T21">
-        <v>0.99072147660779</v>
+        <v>0.9982162562817161</v>
       </c>
       <c r="U21">
-        <v>0.9934934053114188</v>
+        <v>1.000627937214183</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1742,61 +1742,61 @@
         <v>1.03</v>
       </c>
       <c r="C22">
-        <v>1.020206833292289</v>
+        <v>1.020375455738118</v>
       </c>
       <c r="D22">
-        <v>1.012543385164436</v>
+        <v>1.013906984415004</v>
       </c>
       <c r="E22">
-        <v>1.000110769504221</v>
+        <v>1.003301516320825</v>
       </c>
       <c r="F22">
-        <v>0.9995108069481214</v>
+        <v>1.002749840629661</v>
       </c>
       <c r="G22">
-        <v>0.9990876538100957</v>
+        <v>1.002370469817262</v>
       </c>
       <c r="H22">
-        <v>0.9986564561434546</v>
+        <v>1.001941033162741</v>
       </c>
       <c r="I22">
-        <v>0.9981134663582676</v>
+        <v>1.001630551929019</v>
       </c>
       <c r="J22">
-        <v>0.9981678960074742</v>
+        <v>1.001684457490594</v>
       </c>
       <c r="K22">
-        <v>0.9978368860164273</v>
+        <v>1.001389723548368</v>
       </c>
       <c r="L22">
-        <v>0.9973783299491263</v>
+        <v>1.001017078038229</v>
       </c>
       <c r="M22">
-        <v>0.9972836383671657</v>
+        <v>1.000958764392087</v>
       </c>
       <c r="N22">
-        <v>1.021202903668786</v>
+        <v>1.021245955926484</v>
       </c>
       <c r="O22">
-        <v>1.018697866193399</v>
+        <v>1.019643402092265</v>
       </c>
       <c r="P22">
-        <v>1.017796157131988</v>
+        <v>1.018742553682071</v>
       </c>
       <c r="Q22">
-        <v>0.9959398219549739</v>
+        <v>1.001542275684238</v>
       </c>
       <c r="R22">
-        <v>1.01572494281015</v>
+        <v>1.019503169201806</v>
       </c>
       <c r="S22">
-        <v>0.9976555181906851</v>
+        <v>1.002101682440796</v>
       </c>
       <c r="T22">
-        <v>0.9954530890526206</v>
+        <v>1.000816502140914</v>
       </c>
       <c r="U22">
-        <v>0.9988108122067787</v>
+        <v>1.0031595132993</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1807,61 +1807,61 @@
         <v>1.03</v>
       </c>
       <c r="C23">
-        <v>1.02054262197399</v>
+        <v>1.020673386738419</v>
       </c>
       <c r="D23">
-        <v>1.013289246789613</v>
+        <v>1.014380377229865</v>
       </c>
       <c r="E23">
-        <v>1.001486175411977</v>
+        <v>1.004046833582841</v>
       </c>
       <c r="F23">
-        <v>1.000917601146358</v>
+        <v>1.003500408178446</v>
       </c>
       <c r="G23">
-        <v>1.000519560799574</v>
+        <v>1.003122297472079</v>
       </c>
       <c r="H23">
-        <v>1.000101231437502</v>
+        <v>1.002705330080879</v>
       </c>
       <c r="I23">
-        <v>0.9996063609546163</v>
+        <v>1.002435371302353</v>
       </c>
       <c r="J23">
-        <v>0.9996580261270288</v>
+        <v>1.002486622751742</v>
       </c>
       <c r="K23">
-        <v>0.99934352999339</v>
+        <v>1.002202570969344</v>
       </c>
       <c r="L23">
-        <v>0.998915339674924</v>
+        <v>1.00184655625471</v>
       </c>
       <c r="M23">
-        <v>0.998830782035843</v>
+        <v>1.001792585065534</v>
       </c>
       <c r="N23">
-        <v>1.021456364852239</v>
+        <v>1.021479585716867</v>
       </c>
       <c r="O23">
-        <v>1.019322807257644</v>
+        <v>1.019876903148839</v>
       </c>
       <c r="P23">
-        <v>1.018444539036162</v>
+        <v>1.018999126388503</v>
       </c>
       <c r="Q23">
-        <v>0.9978319441769655</v>
+        <v>1.002344529711718</v>
       </c>
       <c r="R23">
-        <v>1.017403221193763</v>
+        <v>1.019612208615851</v>
       </c>
       <c r="S23">
-        <v>0.9994801681804111</v>
+        <v>1.00259929283158</v>
       </c>
       <c r="T23">
-        <v>0.9973982733342519</v>
+        <v>1.001776761182203</v>
       </c>
       <c r="U23">
-        <v>1.00005751404153</v>
+        <v>1.003904912726866</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1872,61 +1872,61 @@
         <v>1.03</v>
       </c>
       <c r="C24">
-        <v>1.021341424696769</v>
+        <v>1.02141591325723</v>
       </c>
       <c r="D24">
-        <v>1.014968999367217</v>
+        <v>1.015641549874597</v>
       </c>
       <c r="E24">
-        <v>1.004521298774415</v>
+        <v>1.006110677680211</v>
       </c>
       <c r="F24">
-        <v>1.003991662369027</v>
+        <v>1.005602421797377</v>
       </c>
       <c r="G24">
-        <v>1.003620355569393</v>
+        <v>1.005250497856304</v>
       </c>
       <c r="H24">
-        <v>1.00323350625451</v>
+        <v>1.004864449035006</v>
       </c>
       <c r="I24">
-        <v>1.002929799982777</v>
+        <v>1.004619785227611</v>
       </c>
       <c r="J24">
-        <v>1.002974707750346</v>
+        <v>1.004664457312333</v>
       </c>
       <c r="K24">
-        <v>1.002702068417455</v>
+        <v>1.004397642763637</v>
       </c>
       <c r="L24">
-        <v>1.002351647656751</v>
+        <v>1.00406066354718</v>
       </c>
       <c r="M24">
-        <v>1.002293368527044</v>
+        <v>1.004007964390359</v>
       </c>
       <c r="N24">
-        <v>1.022045517917197</v>
+        <v>1.022059889098675</v>
       </c>
       <c r="O24">
-        <v>1.020217238135621</v>
+        <v>1.02059753035813</v>
       </c>
       <c r="P24">
-        <v>1.019396331383061</v>
+        <v>1.019776939231271</v>
       </c>
       <c r="Q24">
-        <v>1.002066907743038</v>
+        <v>1.004648588072971</v>
       </c>
       <c r="R24">
-        <v>1.01894306344149</v>
+        <v>1.020457398803088</v>
       </c>
       <c r="S24">
-        <v>1.00258415768755</v>
+        <v>1.004728547089417</v>
       </c>
       <c r="T24">
-        <v>1.001897462270677</v>
+        <v>1.003866039255106</v>
       </c>
       <c r="U24">
-        <v>1.003097008491306</v>
+        <v>1.006094785596281</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -1937,61 +1937,61 @@
         <v>1.03</v>
       </c>
       <c r="C25">
-        <v>1.021716720297421</v>
+        <v>1.021754135059059</v>
       </c>
       <c r="D25">
-        <v>1.015916554672156</v>
+        <v>1.016274825206952</v>
       </c>
       <c r="E25">
-        <v>1.006349250791169</v>
+        <v>1.007200040906886</v>
       </c>
       <c r="F25">
-        <v>1.005857678583578</v>
+        <v>1.006724127681966</v>
       </c>
       <c r="G25">
-        <v>1.005517196884526</v>
+        <v>1.006397889481471</v>
       </c>
       <c r="H25">
-        <v>1.005144666981509</v>
+        <v>1.006025779135655</v>
       </c>
       <c r="I25">
-        <v>1.004857136011943</v>
+        <v>1.005763464679494</v>
       </c>
       <c r="J25">
-        <v>1.004898962841325</v>
+        <v>1.005805167902696</v>
       </c>
       <c r="K25">
-        <v>1.004635534010041</v>
+        <v>1.005547306961417</v>
       </c>
       <c r="L25">
-        <v>1.004296899941357</v>
+        <v>1.005221767299546</v>
       </c>
       <c r="M25">
-        <v>1.004240486460042</v>
+        <v>1.005170869617912</v>
       </c>
       <c r="N25">
-        <v>1.022312534643092</v>
+        <v>1.022319763117604</v>
       </c>
       <c r="O25">
-        <v>1.020732887063272</v>
+        <v>1.020942606382309</v>
       </c>
       <c r="P25">
-        <v>1.019937807660049</v>
+        <v>1.020147695657239</v>
       </c>
       <c r="Q25">
-        <v>1.004504010563682</v>
+        <v>1.005789280637143</v>
       </c>
       <c r="R25">
-        <v>1.020092919670222</v>
+        <v>1.020926480012593</v>
       </c>
       <c r="S25">
-        <v>1.004995377985497</v>
+        <v>1.006256226952764</v>
       </c>
       <c r="T25">
-        <v>1.003845293492152</v>
+        <v>1.005029072429465</v>
       </c>
       <c r="U25">
-        <v>1.005700452727246</v>
+        <v>1.007184131608519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalize presentation, add results of step 4 and cleanup
</commit_message>
<xml_diff>
--- a/PRO1/step_3/results/res_bus/vm_pu.xlsx
+++ b/PRO1/step_3/results/res_bus/vm_pu.xlsx
@@ -442,61 +442,61 @@
         <v>1.03</v>
       </c>
       <c r="C2">
-        <v>1.022285147001913</v>
+        <v>1.022979550322315</v>
       </c>
       <c r="D2">
-        <v>1.01718578158766</v>
+        <v>1.020512189554994</v>
       </c>
       <c r="E2">
-        <v>1.00869958488894</v>
+        <v>1.016147873779704</v>
       </c>
       <c r="F2">
-        <v>1.008251166439402</v>
+        <v>1.015678861854721</v>
       </c>
       <c r="G2">
-        <v>1.007943786846957</v>
+        <v>1.015351673398793</v>
       </c>
       <c r="H2">
-        <v>1.007593967990591</v>
+        <v>1.015005190783635</v>
       </c>
       <c r="I2">
-        <v>1.007360695766427</v>
+        <v>1.01458867923158</v>
       </c>
       <c r="J2">
-        <v>1.007397653642061</v>
+        <v>1.014709297043003</v>
       </c>
       <c r="K2">
-        <v>1.007156767555552</v>
+        <v>1.014449430242089</v>
       </c>
       <c r="L2">
-        <v>1.00685588291752</v>
+        <v>1.014100697196127</v>
       </c>
       <c r="M2">
-        <v>1.006810582744291</v>
+        <v>1.01405650870397</v>
       </c>
       <c r="N2">
-        <v>1.022734980948664</v>
+        <v>1.022718994440795</v>
       </c>
       <c r="O2">
-        <v>1.021430049851221</v>
+        <v>1.021008607494307</v>
       </c>
       <c r="P2">
-        <v>1.02067649724301</v>
+        <v>1.020254733130945</v>
       </c>
       <c r="Q2">
-        <v>1.007381741222288</v>
+        <v>1.019738481939729</v>
       </c>
       <c r="R2">
-        <v>1.021413915781757</v>
+        <v>1.013035421939304</v>
       </c>
       <c r="S2">
-        <v>1.00780229338222</v>
+        <v>1.012270651454535</v>
       </c>
       <c r="T2">
-        <v>1.006794679597638</v>
+        <v>1.010995593342349</v>
       </c>
       <c r="U2">
-        <v>1.008683651904422</v>
+        <v>1.018631723538786</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -507,61 +507,61 @@
         <v>1.03</v>
       </c>
       <c r="C3">
-        <v>1.022651444456785</v>
+        <v>1.023370824948906</v>
       </c>
       <c r="D3">
-        <v>1.017799317063514</v>
+        <v>1.021158231529787</v>
       </c>
       <c r="E3">
-        <v>1.009696498061694</v>
+        <v>1.017189651272366</v>
       </c>
       <c r="F3">
-        <v>1.009267200711153</v>
+        <v>1.016754931894887</v>
       </c>
       <c r="G3">
-        <v>1.00897293623579</v>
+        <v>1.016454795960926</v>
       </c>
       <c r="H3">
-        <v>1.008638619586681</v>
+        <v>1.016123731687082</v>
       </c>
       <c r="I3">
-        <v>1.008418049074436</v>
+        <v>1.015833536765336</v>
       </c>
       <c r="J3">
-        <v>1.008451709632978</v>
+        <v>1.015895277512701</v>
       </c>
       <c r="K3">
-        <v>1.008220790090022</v>
+        <v>1.015656125058111</v>
       </c>
       <c r="L3">
-        <v>1.007932633627258</v>
+        <v>1.015346003911438</v>
       </c>
       <c r="M3">
-        <v>1.007889335253258</v>
+        <v>1.015303812802913</v>
       </c>
       <c r="N3">
-        <v>1.023023459945867</v>
+        <v>1.023013170055216</v>
       </c>
       <c r="O3">
-        <v>1.021768915316444</v>
+        <v>1.021476296645274</v>
       </c>
       <c r="P3">
-        <v>1.021044215156406</v>
+        <v>1.020751381471752</v>
       </c>
       <c r="Q3">
-        <v>1.008435780563791</v>
+        <v>1.020384989979964</v>
       </c>
       <c r="R3">
-        <v>1.021752775894406</v>
+        <v>1.015297723575082</v>
       </c>
       <c r="S3">
-        <v>1.008831555007679</v>
+        <v>1.015056436299179</v>
       </c>
       <c r="T3">
-        <v>1.007873415067094</v>
+        <v>1.01380428141015</v>
       </c>
       <c r="U3">
-        <v>1.009680549330364</v>
+        <v>1.019816202409612</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -572,61 +572,61 @@
         <v>1.03</v>
       </c>
       <c r="C4">
-        <v>1.02303045990309</v>
+        <v>1.023744979948442</v>
       </c>
       <c r="D4">
-        <v>1.018457524839949</v>
+        <v>1.021668523184301</v>
       </c>
       <c r="E4">
-        <v>1.010787487974295</v>
+        <v>1.017893902895499</v>
       </c>
       <c r="F4">
-        <v>1.010382957997341</v>
+        <v>1.01748363661906</v>
       </c>
       <c r="G4">
-        <v>1.010106839196601</v>
+        <v>1.017201436751054</v>
       </c>
       <c r="H4">
-        <v>1.00978854502242</v>
+        <v>1.016886113058096</v>
       </c>
       <c r="I4">
-        <v>1.009571488758209</v>
+        <v>1.01658833492082</v>
       </c>
       <c r="J4">
-        <v>1.009601740039795</v>
+        <v>1.016646721575727</v>
       </c>
       <c r="K4">
-        <v>1.009381117378995</v>
+        <v>1.016415029714107</v>
       </c>
       <c r="L4">
-        <v>1.009106111242643</v>
+        <v>1.016111436860854</v>
       </c>
       <c r="M4">
-        <v>1.009064881192685</v>
+        <v>1.016071277302022</v>
       </c>
       <c r="N4">
-        <v>1.023320448473356</v>
+        <v>1.02331509944485</v>
       </c>
       <c r="O4">
-        <v>1.022117955738541</v>
+        <v>1.021952619260466</v>
       </c>
       <c r="P4">
-        <v>1.021423061652893</v>
+        <v>1.021257608578262</v>
       </c>
       <c r="Q4">
-        <v>1.009585792805222</v>
+        <v>1.02127156288765</v>
       </c>
       <c r="R4">
-        <v>1.022101810803212</v>
+        <v>1.016425330934061</v>
       </c>
       <c r="S4">
-        <v>1.010090883985653</v>
+        <v>1.015811783178083</v>
       </c>
       <c r="T4">
-        <v>1.009048942438102</v>
+        <v>1.014185196474339</v>
       </c>
       <c r="U4">
-        <v>1.010771522010158</v>
+        <v>1.020999765336035</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -637,61 +637,61 @@
         <v>1.03</v>
       </c>
       <c r="C5">
-        <v>1.02303234497713</v>
+        <v>1.023754394077768</v>
       </c>
       <c r="D5">
-        <v>1.018460687785302</v>
+        <v>1.021715102006646</v>
       </c>
       <c r="E5">
-        <v>1.010792633532488</v>
+        <v>1.018034081627411</v>
       </c>
       <c r="F5">
-        <v>1.01038820246331</v>
+        <v>1.017633971256379</v>
       </c>
       <c r="G5">
-        <v>1.010112151498275</v>
+        <v>1.01736104577639</v>
       </c>
       <c r="H5">
-        <v>1.009793937534582</v>
+        <v>1.017045865909692</v>
       </c>
       <c r="I5">
-        <v>1.009576947010709</v>
+        <v>1.016775131258175</v>
       </c>
       <c r="J5">
-        <v>1.009607181232212</v>
+        <v>1.016819789263231</v>
       </c>
       <c r="K5">
-        <v>1.009386610135808</v>
+        <v>1.016593513869732</v>
       </c>
       <c r="L5">
-        <v>1.00911166985086</v>
+        <v>1.016302839867468</v>
       </c>
       <c r="M5">
-        <v>1.009070450157624</v>
+        <v>1.016262700670808</v>
       </c>
       <c r="N5">
-        <v>1.023321936726942</v>
+        <v>1.023316588372004</v>
       </c>
       <c r="O5">
-        <v>1.022119705290602</v>
+        <v>1.021954369814534</v>
       </c>
       <c r="P5">
-        <v>1.021424960830191</v>
+        <v>1.021259508782449</v>
       </c>
       <c r="Q5">
-        <v>1.009591233911692</v>
+        <v>1.020563861581855</v>
       </c>
       <c r="R5">
-        <v>1.022103560327637</v>
+        <v>1.017337601939999</v>
       </c>
       <c r="S5">
-        <v>1.010096196201463</v>
+        <v>1.016376474504589</v>
       </c>
       <c r="T5">
-        <v>1.009054511315077</v>
+        <v>1.015145597709012</v>
       </c>
       <c r="U5">
-        <v>1.010776667487074</v>
+        <v>1.021001517425045</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -702,61 +702,61 @@
         <v>1.03</v>
       </c>
       <c r="C6">
-        <v>1.023273096800444</v>
+        <v>1.023996358832757</v>
       </c>
       <c r="D6">
-        <v>1.018864800887998</v>
+        <v>1.022060439838109</v>
       </c>
       <c r="E6">
-        <v>1.011450228362985</v>
+        <v>1.018504358381998</v>
       </c>
       <c r="F6">
-        <v>1.011058443968306</v>
+        <v>1.0181067281104</v>
       </c>
       <c r="G6">
-        <v>1.010791066721083</v>
+        <v>1.017833196018948</v>
       </c>
       <c r="H6">
-        <v>1.010483108715766</v>
+        <v>1.017528113522309</v>
       </c>
       <c r="I6">
-        <v>1.010274522940922</v>
+        <v>1.017292577641961</v>
       </c>
       <c r="J6">
-        <v>1.010302575830803</v>
+        <v>1.017348763113212</v>
       </c>
       <c r="K6">
-        <v>1.010088597794496</v>
+        <v>1.017136874094088</v>
       </c>
       <c r="L6">
-        <v>1.009822077289054</v>
+        <v>1.016873457521862</v>
       </c>
       <c r="M6">
-        <v>1.00978218181126</v>
+        <v>1.016834626061781</v>
       </c>
       <c r="N6">
-        <v>1.023510875509177</v>
+        <v>1.023505360127946</v>
       </c>
       <c r="O6">
-        <v>1.022301734050026</v>
+        <v>1.02213595554591</v>
       </c>
       <c r="P6">
-        <v>1.021626101731756</v>
+        <v>1.021460209472342</v>
       </c>
       <c r="Q6">
-        <v>1.01028661752613</v>
+        <v>1.021663614695749</v>
       </c>
       <c r="R6">
-        <v>1.022161782947423</v>
+        <v>1.017057549122771</v>
       </c>
       <c r="S6">
-        <v>1.010775100700417</v>
+        <v>1.016516538060372</v>
       </c>
       <c r="T6">
-        <v>1.009766231726507</v>
+        <v>1.016850025115865</v>
       </c>
       <c r="U6">
-        <v>1.011434251930486</v>
+        <v>1.020948801591998</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -767,61 +767,61 @@
         <v>1.03</v>
       </c>
       <c r="C7">
-        <v>1.023082861981823</v>
+        <v>1.023776232687593</v>
       </c>
       <c r="D7">
-        <v>1.018522879991381</v>
+        <v>1.021597954284243</v>
       </c>
       <c r="E7">
-        <v>1.010873233699438</v>
+        <v>1.017701386841225</v>
       </c>
       <c r="F7">
-        <v>1.010471547589995</v>
+        <v>1.017273518890578</v>
       </c>
       <c r="G7">
-        <v>1.010197379171471</v>
+        <v>1.016974558570464</v>
       </c>
       <c r="H7">
-        <v>1.009881390676519</v>
+        <v>1.016661392845021</v>
       </c>
       <c r="I7">
-        <v>1.009666221449531</v>
+        <v>1.016277051791415</v>
       </c>
       <c r="J7">
-        <v>1.009695984590893</v>
+        <v>1.016418603100391</v>
       </c>
       <c r="K7">
-        <v>1.009476845125709</v>
+        <v>1.016193622897835</v>
       </c>
       <c r="L7">
-        <v>1.009203732727853</v>
+        <v>1.015904595738295</v>
       </c>
       <c r="M7">
-        <v>1.009162800392238</v>
+        <v>1.015864715454744</v>
       </c>
       <c r="N7">
-        <v>1.023363719215658</v>
+        <v>1.023338511056912</v>
       </c>
       <c r="O7">
-        <v>1.022168825642667</v>
+        <v>1.021532130492994</v>
       </c>
       <c r="P7">
-        <v>1.021478283003365</v>
+        <v>1.02084114138866</v>
       </c>
       <c r="Q7">
-        <v>1.009680035867673</v>
+        <v>1.020446584628799</v>
       </c>
       <c r="R7">
-        <v>1.022152679903884</v>
+        <v>1.01466207585446</v>
       </c>
       <c r="S7">
-        <v>1.010181422528439</v>
+        <v>1.013178851134528</v>
       </c>
       <c r="T7">
-        <v>1.009146860090967</v>
+        <v>1.014746909262458</v>
       </c>
       <c r="U7">
-        <v>1.010732059023049</v>
+        <v>1.017943909551186</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -832,61 +832,61 @@
         <v>1.03</v>
       </c>
       <c r="C8">
-        <v>1.022628219223735</v>
+        <v>1.023336195792807</v>
       </c>
       <c r="D8">
-        <v>1.017760394738771</v>
+        <v>1.021055935463685</v>
       </c>
       <c r="E8">
-        <v>1.009633231514454</v>
+        <v>1.017000374265078</v>
       </c>
       <c r="F8">
-        <v>1.009202719842634</v>
+        <v>1.016559318275545</v>
       </c>
       <c r="G8">
-        <v>1.008907622464649</v>
+        <v>1.016253665825632</v>
       </c>
       <c r="H8">
-        <v>1.00857232132004</v>
+        <v>1.015921565678796</v>
       </c>
       <c r="I8">
-        <v>1.008350944295946</v>
+        <v>1.015552185402381</v>
       </c>
       <c r="J8">
-        <v>1.008384814253474</v>
+        <v>1.015669661371329</v>
       </c>
       <c r="K8">
-        <v>1.008153261783636</v>
+        <v>1.015432493503618</v>
       </c>
       <c r="L8">
-        <v>1.00786429701981</v>
+        <v>1.015127898106641</v>
       </c>
       <c r="M8">
-        <v>1.007820871521551</v>
+        <v>1.015085572330863</v>
       </c>
       <c r="N8">
-        <v>1.023005156338313</v>
+        <v>1.022983566802035</v>
       </c>
       <c r="O8">
-        <v>1.021747409679759</v>
+        <v>1.021196854966506</v>
       </c>
       <c r="P8">
-        <v>1.021020875965341</v>
+        <v>1.020469915609171</v>
       </c>
       <c r="Q8">
-        <v>1.008368886240937</v>
+        <v>1.019903967623313</v>
       </c>
       <c r="R8">
-        <v>1.021731270597415</v>
+        <v>1.014713313971942</v>
       </c>
       <c r="S8">
-        <v>1.008766234123949</v>
+        <v>1.013236400313155</v>
       </c>
       <c r="T8">
-        <v>1.007804952416811</v>
+        <v>1.013969344105661</v>
       </c>
       <c r="U8">
-        <v>1.009617283783582</v>
+        <v>1.018095600011378</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -897,61 +897,61 @@
         <v>1.03</v>
       </c>
       <c r="C9">
-        <v>1.021363486022933</v>
+        <v>1.022076537383953</v>
       </c>
       <c r="D9">
-        <v>1.015645085283198</v>
+        <v>1.019344251112536</v>
       </c>
       <c r="E9">
-        <v>1.006199523560017</v>
+        <v>1.014603720056614</v>
       </c>
       <c r="F9">
-        <v>1.005703277769442</v>
+        <v>1.014103069554501</v>
       </c>
       <c r="G9">
-        <v>1.005363093886676</v>
+        <v>1.013757707917539</v>
       </c>
       <c r="H9">
-        <v>1.004974499376951</v>
+        <v>1.013373219975865</v>
       </c>
       <c r="I9">
-        <v>1.004709436670169</v>
+        <v>1.012931909890254</v>
       </c>
       <c r="J9">
-        <v>1.004754642571241</v>
+        <v>1.013046700855961</v>
       </c>
       <c r="K9">
-        <v>1.004488824761512</v>
+        <v>1.012765056321067</v>
       </c>
       <c r="L9">
-        <v>1.004156099521488</v>
+        <v>1.012391537296284</v>
       </c>
       <c r="M9">
-        <v>1.004105791718521</v>
+        <v>1.012342438749518</v>
       </c>
       <c r="N9">
-        <v>1.022010969472217</v>
+        <v>1.021992103249435</v>
       </c>
       <c r="O9">
-        <v>1.020580323946096</v>
+        <v>1.020114393783838</v>
       </c>
       <c r="P9">
-        <v>1.019754784223464</v>
+        <v>1.019288465053763</v>
       </c>
       <c r="Q9">
-        <v>1.004738771899334</v>
+        <v>1.017808550409023</v>
       </c>
       <c r="R9">
-        <v>1.020564203298537</v>
+        <v>1.012597620088475</v>
       </c>
       <c r="S9">
-        <v>1.00522131781511</v>
+        <v>1.010999568301723</v>
       </c>
       <c r="T9">
-        <v>1.004089931295582</v>
+        <v>1.009675992996959</v>
       </c>
       <c r="U9">
-        <v>1.006183630065392</v>
+        <v>1.017494494186339</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -962,61 +962,61 @@
         <v>1.03</v>
       </c>
       <c r="C10">
-        <v>1.016814234525497</v>
+        <v>1.017568297457729</v>
       </c>
       <c r="D10">
-        <v>1.008122392769343</v>
+        <v>1.01332016723603</v>
       </c>
       <c r="E10">
-        <v>0.9940787794780779</v>
+        <v>1.006280088799027</v>
       </c>
       <c r="F10">
-        <v>0.9933569635440676</v>
+        <v>1.005548663317946</v>
       </c>
       <c r="G10">
-        <v>0.9928632470425371</v>
+        <v>1.005043829903653</v>
       </c>
       <c r="H10">
-        <v>0.9922876376532933</v>
+        <v>1.004476490355704</v>
       </c>
       <c r="I10">
-        <v>0.9918590550176537</v>
+        <v>1.003867718495713</v>
       </c>
       <c r="J10">
-        <v>0.9919440492234762</v>
+        <v>1.00403606707086</v>
       </c>
       <c r="K10">
-        <v>0.9915579309088464</v>
+        <v>1.003636545646235</v>
       </c>
       <c r="L10">
-        <v>0.9910715578341366</v>
+        <v>1.003112293193919</v>
       </c>
       <c r="M10">
-        <v>0.9909970864997705</v>
+        <v>1.003039559853758</v>
       </c>
       <c r="N10">
-        <v>1.018471851288541</v>
+        <v>1.018429539861765</v>
       </c>
       <c r="O10">
-        <v>1.016441188574724</v>
+        <v>1.015657569077207</v>
       </c>
       <c r="P10">
-        <v>1.015272061620074</v>
+        <v>1.014487518913813</v>
       </c>
       <c r="Q10">
-        <v>0.9919283809021879</v>
+        <v>1.010607185217149</v>
       </c>
       <c r="R10">
-        <v>1.016425133307166</v>
+        <v>1.003486354262181</v>
       </c>
       <c r="S10">
-        <v>0.9928475642019957</v>
+        <v>1.001524425840447</v>
       </c>
       <c r="T10">
-        <v>0.9909814331362977</v>
+        <v>1.000370864638326</v>
       </c>
       <c r="U10">
-        <v>0.994063077437509</v>
+        <v>1.011303164771764</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1027,61 +1027,61 @@
         <v>1.03</v>
       </c>
       <c r="C11">
-        <v>1.012579261596185</v>
+        <v>1.013397391101579</v>
       </c>
       <c r="D11">
-        <v>1.001129543381241</v>
+        <v>1.007807841079202</v>
       </c>
       <c r="E11">
-        <v>0.9828381145814301</v>
+        <v>0.9986147611407246</v>
       </c>
       <c r="F11">
-        <v>0.981904212223619</v>
+        <v>0.9976721389952554</v>
       </c>
       <c r="G11">
-        <v>0.9812638691735526</v>
+        <v>0.9970200457216564</v>
       </c>
       <c r="H11">
-        <v>0.9805204341534941</v>
+        <v>0.996290040452643</v>
       </c>
       <c r="I11">
-        <v>0.9799631021533421</v>
+        <v>0.9955078761988757</v>
       </c>
       <c r="J11">
-        <v>0.9800838190275935</v>
+        <v>0.9957114621049442</v>
       </c>
       <c r="K11">
-        <v>0.9795896827800931</v>
+        <v>0.9951929648907416</v>
       </c>
       <c r="L11">
-        <v>0.9789653319238952</v>
+        <v>0.994500796172326</v>
       </c>
       <c r="M11">
-        <v>0.978869162257457</v>
+        <v>0.9944070132281793</v>
       </c>
       <c r="N11">
-        <v>1.015240276294989</v>
+        <v>1.015203979565415</v>
       </c>
       <c r="O11">
-        <v>1.012681064882455</v>
+        <v>1.012068238695784</v>
       </c>
       <c r="P11">
-        <v>1.011209271566259</v>
+        <v>1.010595536620757</v>
       </c>
       <c r="Q11">
-        <v>0.9800683380453971</v>
+        <v>1.006641041943841</v>
       </c>
       <c r="R11">
-        <v>1.012665069008192</v>
+        <v>0.9946603114663206</v>
       </c>
       <c r="S11">
-        <v>0.9811193715294363</v>
+        <v>0.9931444784967178</v>
       </c>
       <c r="T11">
-        <v>0.9788537004614561</v>
+        <v>0.98969284992845</v>
       </c>
       <c r="U11">
-        <v>0.9826937993875019</v>
+        <v>1.008691878856177</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1092,61 +1092,61 @@
         <v>1.03</v>
       </c>
       <c r="C12">
-        <v>1.005270789924841</v>
+        <v>1.006069869722698</v>
       </c>
       <c r="D12">
-        <v>0.9892122949438726</v>
+        <v>0.9978870999955158</v>
       </c>
       <c r="E12">
-        <v>0.9638550446444304</v>
+        <v>0.9847078609305376</v>
       </c>
       <c r="F12">
-        <v>0.9625619972372293</v>
+        <v>0.9833684768995853</v>
       </c>
       <c r="G12">
-        <v>0.9616717244623377</v>
+        <v>0.9824290832618399</v>
       </c>
       <c r="H12">
-        <v>0.9606499612668414</v>
+        <v>0.9814311486805847</v>
       </c>
       <c r="I12">
-        <v>0.959880749307347</v>
+        <v>0.9800993210664142</v>
       </c>
       <c r="J12">
-        <v>0.9600607346844061</v>
+        <v>0.98057263060194</v>
       </c>
       <c r="K12">
-        <v>0.9593845271472139</v>
+        <v>0.9798631420663763</v>
       </c>
       <c r="L12">
-        <v>0.9585244489847523</v>
+        <v>0.9789065558963966</v>
       </c>
       <c r="M12">
-        <v>0.9583894080726866</v>
+        <v>0.9787780563516725</v>
       </c>
       <c r="N12">
-        <v>1.009783371471103</v>
+        <v>1.009711040821022</v>
       </c>
       <c r="O12">
-        <v>1.006368473770558</v>
+        <v>1.005417860089497</v>
       </c>
       <c r="P12">
-        <v>1.004406674851278</v>
+        <v>1.003454175750863</v>
       </c>
       <c r="Q12">
-        <v>0.9600455699782323</v>
+        <v>0.9963184794310022</v>
       </c>
       <c r="R12">
-        <v>1.006352577607267</v>
+        <v>0.9749764412952012</v>
       </c>
       <c r="S12">
-        <v>0.9611272144318036</v>
+        <v>0.9717399323597344</v>
       </c>
       <c r="T12">
-        <v>0.9582421821020901</v>
+        <v>0.9714238285139711</v>
       </c>
       <c r="U12">
-        <v>0.9638398200049691</v>
+        <v>1.000253636410484</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1157,61 +1157,61 @@
         <v>1.03</v>
       </c>
       <c r="C13">
-        <v>0.9991679966197937</v>
+        <v>1.00019115156633</v>
       </c>
       <c r="D13">
-        <v>0.979431634999295</v>
+        <v>0.9903757546799835</v>
       </c>
       <c r="E13">
-        <v>0.9484622593957603</v>
+        <v>0.9748111594539235</v>
       </c>
       <c r="F13">
-        <v>0.9468983952154666</v>
+        <v>0.9732160583427176</v>
       </c>
       <c r="G13">
-        <v>0.945823617863402</v>
+        <v>0.972102427319635</v>
       </c>
       <c r="H13">
-        <v>0.9445781079160566</v>
+        <v>0.9708934566122018</v>
       </c>
       <c r="I13">
-        <v>0.9436004224575046</v>
+        <v>0.9696111110947958</v>
       </c>
       <c r="J13">
-        <v>0.9438280814380111</v>
+        <v>0.9700237376893482</v>
       </c>
       <c r="K13">
-        <v>0.9430103344577621</v>
+        <v>0.9691894785760052</v>
       </c>
       <c r="L13">
-        <v>0.9419725211111718</v>
+        <v>0.9680862376233539</v>
       </c>
       <c r="M13">
-        <v>0.941811338369978</v>
+        <v>0.9679304088409469</v>
       </c>
       <c r="N13">
-        <v>1.005317269659471</v>
+        <v>1.005120971401468</v>
       </c>
       <c r="O13">
-        <v>1.001150612926383</v>
+        <v>0.9991854105433872</v>
       </c>
       <c r="P13">
-        <v>0.9988054745375345</v>
+        <v>0.9968355896410496</v>
       </c>
       <c r="Q13">
-        <v>0.9435444178233119</v>
+        <v>0.9859622894654333</v>
       </c>
       <c r="R13">
-        <v>1.000881534605665</v>
+        <v>0.9650042513545661</v>
       </c>
       <c r="S13">
-        <v>0.9454056715128591</v>
+        <v>0.9642408493145235</v>
       </c>
       <c r="T13">
-        <v>0.9417964619234142</v>
+        <v>0.9622735205189902</v>
       </c>
       <c r="U13">
-        <v>0.9484472778941104</v>
+        <v>0.9880499108880089</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1222,61 +1222,61 @@
         <v>1.03</v>
       </c>
       <c r="C14">
-        <v>0.9986046686511212</v>
+        <v>0.9996229380704637</v>
       </c>
       <c r="D14">
-        <v>0.9785818487264724</v>
+        <v>0.9896347210664052</v>
       </c>
       <c r="E14">
-        <v>0.9471744317449415</v>
+        <v>0.9738235798465855</v>
       </c>
       <c r="F14">
-        <v>0.9455958948862359</v>
+        <v>0.9721868272054245</v>
       </c>
       <c r="G14">
-        <v>0.9445135280564046</v>
+        <v>0.9710406502097778</v>
       </c>
       <c r="H14">
-        <v>0.9432473928108169</v>
+        <v>0.9698120040568576</v>
       </c>
       <c r="I14">
-        <v>0.9422315737003187</v>
+        <v>0.9685823329682385</v>
       </c>
       <c r="J14">
-        <v>0.9424636290050548</v>
+        <v>0.968999335537549</v>
       </c>
       <c r="K14">
-        <v>0.9416297166770886</v>
+        <v>0.9681612200374862</v>
       </c>
       <c r="L14">
-        <v>0.9405680661886365</v>
+        <v>0.9670629140182877</v>
       </c>
       <c r="M14">
-        <v>0.9404012977539142</v>
+        <v>0.9669045514322466</v>
       </c>
       <c r="N14">
-        <v>1.004901796579473</v>
+        <v>1.004748196218916</v>
       </c>
       <c r="O14">
-        <v>1.000714956550834</v>
+        <v>0.9991070025617889</v>
       </c>
       <c r="P14">
-        <v>0.9983346761872731</v>
+        <v>0.9967228335086398</v>
       </c>
       <c r="Q14">
-        <v>0.9423144144727951</v>
+        <v>0.9848013791731016</v>
       </c>
       <c r="R14">
-        <v>1.000572667243163</v>
+        <v>0.9625924792602839</v>
       </c>
       <c r="S14">
-        <v>0.9443645737489411</v>
+        <v>0.9632058740307581</v>
       </c>
       <c r="T14">
-        <v>0.9402518201331235</v>
+        <v>0.9625356603663618</v>
       </c>
       <c r="U14">
-        <v>0.947159470585263</v>
+        <v>0.9901921190702433</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1287,61 +1287,61 @@
         <v>1.03</v>
       </c>
       <c r="C15">
-        <v>0.9990691112048488</v>
+        <v>1.000035427008473</v>
       </c>
       <c r="D15">
-        <v>0.979298664546455</v>
+        <v>0.9901108503691363</v>
       </c>
       <c r="E15">
-        <v>0.9482764669429721</v>
+        <v>0.9743030233678376</v>
       </c>
       <c r="F15">
-        <v>0.9467187628932123</v>
+        <v>0.97269708138556</v>
       </c>
       <c r="G15">
-        <v>0.9456506791649187</v>
+        <v>0.9715746907166739</v>
       </c>
       <c r="H15">
-        <v>0.9444014367413697</v>
+        <v>0.9703616132019083</v>
       </c>
       <c r="I15">
-        <v>0.9434113385908947</v>
+        <v>0.9688793419790812</v>
       </c>
       <c r="J15">
-        <v>0.9436397926515715</v>
+        <v>0.9694021455026198</v>
       </c>
       <c r="K15">
-        <v>0.9428167966706984</v>
+        <v>0.9685621616751866</v>
       </c>
       <c r="L15">
-        <v>0.941769099804964</v>
+        <v>0.9674482336849101</v>
       </c>
       <c r="M15">
-        <v>0.941604527438661</v>
+        <v>0.9672918548405421</v>
       </c>
       <c r="N15">
-        <v>1.005236113519161</v>
+        <v>1.00505516517262</v>
       </c>
       <c r="O15">
-        <v>1.001016555066448</v>
+        <v>0.9991976897712899</v>
       </c>
       <c r="P15">
-        <v>0.9986647528673597</v>
+        <v>0.9968415415480502</v>
       </c>
       <c r="Q15">
-        <v>0.9436248873265533</v>
+        <v>0.9873322735091937</v>
       </c>
       <c r="R15">
-        <v>1.000620179481709</v>
+        <v>0.9640285165422</v>
       </c>
       <c r="S15">
-        <v>0.9455018686515984</v>
+        <v>0.9604096934905181</v>
       </c>
       <c r="T15">
-        <v>0.941455203467457</v>
+        <v>0.9611946236867076</v>
       </c>
       <c r="U15">
-        <v>0.9479940029316447</v>
+        <v>0.9886245306630761</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1352,61 +1352,61 @@
         <v>1.03</v>
       </c>
       <c r="C16">
-        <v>0.9990990217988024</v>
+        <v>1.000032459816178</v>
       </c>
       <c r="D16">
-        <v>0.9793946597972771</v>
+        <v>0.9900734503570565</v>
       </c>
       <c r="E16">
-        <v>0.9484711443899461</v>
+        <v>0.9742701723191899</v>
       </c>
       <c r="F16">
-        <v>0.9469143515071947</v>
+        <v>0.9726761816801681</v>
       </c>
       <c r="G16">
-        <v>0.9458468928185623</v>
+        <v>0.9715646074307639</v>
       </c>
       <c r="H16">
-        <v>0.944598389969418</v>
+        <v>0.9703519626292881</v>
       </c>
       <c r="I16">
-        <v>0.9436089209881274</v>
+        <v>0.9688392820513771</v>
       </c>
       <c r="J16">
-        <v>0.9438372122168404</v>
+        <v>0.9693461880144146</v>
       </c>
       <c r="K16">
-        <v>0.9430146921242556</v>
+        <v>0.9684974225959767</v>
       </c>
       <c r="L16">
-        <v>0.9419676050562454</v>
+        <v>0.9673621477485436</v>
       </c>
       <c r="M16">
-        <v>0.9418031292276379</v>
+        <v>0.9672058113497981</v>
       </c>
       <c r="N16">
-        <v>1.005253026490274</v>
+        <v>1.005083452618092</v>
       </c>
       <c r="O16">
-        <v>1.001117812489742</v>
+        <v>0.9993614590811533</v>
       </c>
       <c r="P16">
-        <v>0.9987670867751097</v>
+        <v>0.997006539305443</v>
       </c>
       <c r="Q16">
-        <v>0.943822303770445</v>
+        <v>0.9860718420868023</v>
       </c>
       <c r="R16">
-        <v>1.000975567881905</v>
+        <v>0.9649026536380713</v>
       </c>
       <c r="S16">
-        <v>0.945698107078547</v>
+        <v>0.960820762238255</v>
       </c>
       <c r="T16">
-        <v>0.9416538305754691</v>
+        <v>0.9597790058554412</v>
       </c>
       <c r="U16">
-        <v>0.9484561627500085</v>
+        <v>0.9896248513426043</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1417,61 +1417,61 @@
         <v>1.03</v>
       </c>
       <c r="C17">
-        <v>0.999136841114627</v>
+        <v>0.9999597960194725</v>
       </c>
       <c r="D17">
-        <v>0.9793825595764196</v>
+        <v>0.9897948322022689</v>
       </c>
       <c r="E17">
-        <v>0.9483859449904951</v>
+        <v>0.9737157903937602</v>
       </c>
       <c r="F17">
-        <v>0.9468206652184485</v>
+        <v>0.9721345643122864</v>
       </c>
       <c r="G17">
-        <v>0.9457449171299841</v>
+        <v>0.9710343259586307</v>
       </c>
       <c r="H17">
-        <v>0.944498260079398</v>
+        <v>0.9698228998279248</v>
       </c>
       <c r="I17">
-        <v>0.9435426901048459</v>
+        <v>0.9679356160084442</v>
       </c>
       <c r="J17">
-        <v>0.9437705856444407</v>
+        <v>0.9686049662558842</v>
       </c>
       <c r="K17">
-        <v>0.9429521193889016</v>
+        <v>0.9677414017914353</v>
       </c>
       <c r="L17">
-        <v>0.9419133870583388</v>
+        <v>0.9665699154762253</v>
       </c>
       <c r="M17">
-        <v>0.9417520598761547</v>
+        <v>0.966413689689558</v>
       </c>
       <c r="N17">
-        <v>1.005297486013601</v>
+        <v>1.005156626661522</v>
       </c>
       <c r="O17">
-        <v>1.001168817478008</v>
+        <v>0.9996627578098196</v>
       </c>
       <c r="P17">
-        <v>0.9988218388827838</v>
+        <v>0.9973121896239592</v>
       </c>
       <c r="Q17">
-        <v>0.9437556782504501</v>
+        <v>0.9849623303652973</v>
       </c>
       <c r="R17">
-        <v>1.001026578525464</v>
+        <v>0.965240914935018</v>
       </c>
       <c r="S17">
-        <v>0.9453269381237015</v>
+        <v>0.9552437226229077</v>
       </c>
       <c r="T17">
-        <v>0.9417371843662482</v>
+        <v>0.9566994127810645</v>
       </c>
       <c r="U17">
-        <v>0.9481035103465146</v>
+        <v>0.9912972561936612</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1482,61 +1482,61 @@
         <v>1.03</v>
       </c>
       <c r="C18">
-        <v>1.004996666910926</v>
+        <v>1.005696234605905</v>
       </c>
       <c r="D18">
-        <v>0.9887478331778264</v>
+        <v>0.9972032761225743</v>
       </c>
       <c r="E18">
-        <v>0.963100394624579</v>
+        <v>0.9836797661365848</v>
       </c>
       <c r="F18">
-        <v>0.961800226376054</v>
+        <v>0.9823277416098415</v>
       </c>
       <c r="G18">
-        <v>0.9609062886662625</v>
+        <v>0.9813796557709155</v>
       </c>
       <c r="H18">
-        <v>0.9598744566290048</v>
+        <v>0.9803715608564809</v>
       </c>
       <c r="I18">
-        <v>0.9590980536539537</v>
+        <v>0.9787937120130801</v>
       </c>
       <c r="J18">
-        <v>0.9592801853580394</v>
+        <v>0.9793814273331587</v>
       </c>
       <c r="K18">
-        <v>0.9586002669842554</v>
+        <v>0.9786561922236818</v>
       </c>
       <c r="L18">
-        <v>0.9577385681054665</v>
+        <v>0.9776692518409474</v>
       </c>
       <c r="M18">
-        <v>0.9576050759620441</v>
+        <v>0.9775394122121772</v>
       </c>
       <c r="N18">
-        <v>1.009585311052823</v>
+        <v>1.009398121825193</v>
       </c>
       <c r="O18">
-        <v>1.006140152316455</v>
+        <v>1.004068040127287</v>
       </c>
       <c r="P18">
-        <v>1.004161024335808</v>
+        <v>1.002084760812032</v>
       </c>
       <c r="Q18">
-        <v>0.9592650329810867</v>
+        <v>0.9928220131878105</v>
       </c>
       <c r="R18">
-        <v>1.006124259759632</v>
+        <v>0.973918077413188</v>
       </c>
       <c r="S18">
-        <v>0.9604944969778623</v>
+        <v>0.9672153579395434</v>
       </c>
       <c r="T18">
-        <v>0.9575899500443986</v>
+        <v>0.9688368157993115</v>
       </c>
       <c r="U18">
-        <v>0.9626894813223259</v>
+        <v>0.9927153900929324</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1547,61 +1547,61 @@
         <v>1.03</v>
       </c>
       <c r="C19">
-        <v>1.014631993067221</v>
+        <v>1.015049929582345</v>
       </c>
       <c r="D19">
-        <v>1.004395882194901</v>
+        <v>1.009116426845557</v>
       </c>
       <c r="E19">
-        <v>0.9879745040824554</v>
+        <v>0.9996442062868822</v>
       </c>
       <c r="F19">
-        <v>0.9871408362181683</v>
+        <v>0.9986920094579838</v>
       </c>
       <c r="G19">
-        <v>0.9865692324945922</v>
+        <v>0.9980093218275767</v>
       </c>
       <c r="H19">
-        <v>0.9859070657021238</v>
+        <v>0.9973559647297071</v>
       </c>
       <c r="I19">
-        <v>0.9854058989132322</v>
+        <v>0.9959644128526186</v>
       </c>
       <c r="J19">
-        <v>0.9855093292498712</v>
+        <v>0.9965330127063508</v>
       </c>
       <c r="K19">
-        <v>0.9850675102888944</v>
+        <v>0.9960165878740307</v>
       </c>
       <c r="L19">
-        <v>0.9845099871279789</v>
+        <v>0.9952739164905907</v>
       </c>
       <c r="M19">
-        <v>0.9844243259524126</v>
+        <v>0.9951900036914622</v>
       </c>
       <c r="N19">
-        <v>1.016814662975463</v>
+        <v>1.016574579881137</v>
       </c>
       <c r="O19">
-        <v>1.014470401983127</v>
+        <v>1.011641184571151</v>
       </c>
       <c r="P19">
-        <v>1.013144948709212</v>
+        <v>1.010311945615634</v>
       </c>
       <c r="Q19">
-        <v>0.985365322118458</v>
+        <v>1.002727752381052</v>
       </c>
       <c r="R19">
-        <v>1.014329615859043</v>
+        <v>0.9876019424631944</v>
       </c>
       <c r="S19">
-        <v>0.9864253470701912</v>
+        <v>0.982765918835282</v>
       </c>
       <c r="T19">
-        <v>0.9844087764094366</v>
+        <v>0.9834622632344013</v>
       </c>
       <c r="U19">
-        <v>0.9874438603245242</v>
+        <v>0.9954888207348904</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1612,61 +1612,61 @@
         <v>1.03</v>
       </c>
       <c r="C20">
-        <v>1.016993975185224</v>
+        <v>1.017552828708938</v>
       </c>
       <c r="D20">
-        <v>1.008211905452195</v>
+        <v>1.012707852232571</v>
       </c>
       <c r="E20">
-        <v>0.9940333645651582</v>
+        <v>1.004822311304552</v>
       </c>
       <c r="F20">
-        <v>0.9933063813733618</v>
+        <v>1.004002775320681</v>
       </c>
       <c r="G20">
-        <v>0.9928055834822076</v>
+        <v>1.003415155485051</v>
       </c>
       <c r="H20">
-        <v>0.9922382036366644</v>
+        <v>1.002854902328639</v>
       </c>
       <c r="I20">
-        <v>0.9918130432827641</v>
+        <v>1.001848993639815</v>
       </c>
       <c r="J20">
-        <v>0.9918963091956718</v>
+        <v>1.002268388130439</v>
       </c>
       <c r="K20">
-        <v>0.9915128135876136</v>
+        <v>1.001839396359162</v>
       </c>
       <c r="L20">
-        <v>0.9910267678671212</v>
+        <v>1.001239209595789</v>
       </c>
       <c r="M20">
-        <v>0.9909506023243406</v>
+        <v>1.001167368297894</v>
       </c>
       <c r="N20">
-        <v>1.018633813574398</v>
+        <v>1.018463660158887</v>
       </c>
       <c r="O20">
-        <v>1.016549455756345</v>
+        <v>1.014289376673885</v>
       </c>
       <c r="P20">
-        <v>1.015396012111086</v>
+        <v>1.013133301893263</v>
       </c>
       <c r="Q20">
-        <v>0.9916249985896779</v>
+        <v>1.008397924895407</v>
       </c>
       <c r="R20">
-        <v>1.016283994988764</v>
+        <v>0.9944030916438473</v>
       </c>
       <c r="S20">
-        <v>0.9924061591949507</v>
+        <v>0.9923794493503431</v>
       </c>
       <c r="T20">
-        <v>0.990807216847349</v>
+        <v>0.9935127084496918</v>
       </c>
       <c r="U20">
-        <v>0.9936343995357819</v>
+        <v>1.001100690266364</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1677,61 +1677,61 @@
         <v>1.03</v>
       </c>
       <c r="C21">
-        <v>1.019480750293981</v>
+        <v>1.019895705263288</v>
       </c>
       <c r="D21">
-        <v>1.012419505188322</v>
+        <v>1.015563119237709</v>
       </c>
       <c r="E21">
-        <v>1.000897076100353</v>
+        <v>1.008454676029138</v>
       </c>
       <c r="F21">
-        <v>1.00030482731351</v>
+        <v>1.007722441082852</v>
       </c>
       <c r="G21">
-        <v>0.999898796933354</v>
+        <v>1.007186922120343</v>
       </c>
       <c r="H21">
-        <v>0.9994323664950373</v>
+        <v>1.006724640346661</v>
       </c>
       <c r="I21">
-        <v>0.9990817246871758</v>
+        <v>1.005509372860097</v>
       </c>
       <c r="J21">
-        <v>0.99914350182752</v>
+        <v>1.006080669749073</v>
       </c>
       <c r="K21">
-        <v>0.9988249638212937</v>
+        <v>1.005703251391523</v>
       </c>
       <c r="L21">
-        <v>0.9984219084762803</v>
+        <v>1.00515597711337</v>
       </c>
       <c r="M21">
-        <v>0.9983588078465327</v>
+        <v>1.005096792374623</v>
       </c>
       <c r="N21">
-        <v>1.020548749580749</v>
+        <v>1.020325379145831</v>
       </c>
       <c r="O21">
-        <v>1.018827125290082</v>
+        <v>1.01593804281365</v>
       </c>
       <c r="P21">
-        <v>1.01785811274824</v>
+        <v>1.014966198937223</v>
       </c>
       <c r="Q21">
-        <v>0.9990010377626097</v>
+        <v>1.011667546714844</v>
       </c>
       <c r="R21">
-        <v>1.018686805532224</v>
+        <v>0.9955407079504542</v>
       </c>
       <c r="S21">
-        <v>0.9997564169413224</v>
+        <v>0.9910570447006375</v>
       </c>
       <c r="T21">
-        <v>0.9982162562817161</v>
+        <v>0.9957222663855767</v>
       </c>
       <c r="U21">
-        <v>1.000627937214183</v>
+        <v>0.9992765130001782</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1742,61 +1742,61 @@
         <v>1.03</v>
       </c>
       <c r="C22">
-        <v>1.020375455738118</v>
+        <v>1.020927940775509</v>
       </c>
       <c r="D22">
-        <v>1.013906984415004</v>
+        <v>1.017253569890893</v>
       </c>
       <c r="E22">
-        <v>1.003301516320825</v>
+        <v>1.011145174358586</v>
       </c>
       <c r="F22">
-        <v>1.002749840629661</v>
+        <v>1.010487287229293</v>
       </c>
       <c r="G22">
-        <v>1.002370469817262</v>
+        <v>1.010009409204983</v>
       </c>
       <c r="H22">
-        <v>1.001941033162741</v>
+        <v>1.009584030307982</v>
       </c>
       <c r="I22">
-        <v>1.001630551929019</v>
+        <v>1.008758571558013</v>
       </c>
       <c r="J22">
-        <v>1.001684457490594</v>
+        <v>1.009162146855098</v>
       </c>
       <c r="K22">
-        <v>1.001389723548368</v>
+        <v>1.008840327205547</v>
       </c>
       <c r="L22">
-        <v>1.001017078038229</v>
+        <v>1.008399869335386</v>
       </c>
       <c r="M22">
-        <v>1.000958764392087</v>
+        <v>1.008345477761919</v>
       </c>
       <c r="N22">
-        <v>1.021245955926484</v>
+        <v>1.021080436776212</v>
       </c>
       <c r="O22">
-        <v>1.019643402092265</v>
+        <v>1.017266281161573</v>
       </c>
       <c r="P22">
-        <v>1.018742553682071</v>
+        <v>1.016363266022155</v>
       </c>
       <c r="Q22">
-        <v>1.001542275684238</v>
+        <v>1.013762938403008</v>
       </c>
       <c r="R22">
-        <v>1.019503169201806</v>
+        <v>1.000627774379914</v>
       </c>
       <c r="S22">
-        <v>1.002101682440796</v>
+        <v>0.9989232947621308</v>
       </c>
       <c r="T22">
-        <v>1.000816502140914</v>
+        <v>1.003662948428617</v>
       </c>
       <c r="U22">
-        <v>1.0031595132993</v>
+        <v>1.003553373481552</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1807,61 +1807,61 @@
         <v>1.03</v>
       </c>
       <c r="C23">
-        <v>1.020673386738419</v>
+        <v>1.021260848833292</v>
       </c>
       <c r="D23">
-        <v>1.014380377229865</v>
+        <v>1.017767912819295</v>
       </c>
       <c r="E23">
-        <v>1.004046833582841</v>
+        <v>1.01197815867265</v>
       </c>
       <c r="F23">
-        <v>1.003500408178446</v>
+        <v>1.011374290238642</v>
       </c>
       <c r="G23">
-        <v>1.003122297472079</v>
+        <v>1.010942384546121</v>
       </c>
       <c r="H23">
-        <v>1.002705330080879</v>
+        <v>1.01052947128489</v>
       </c>
       <c r="I23">
-        <v>1.002435371302353</v>
+        <v>1.009715160114127</v>
       </c>
       <c r="J23">
-        <v>1.002486622751742</v>
+        <v>1.010054715372944</v>
       </c>
       <c r="K23">
-        <v>1.002202570969344</v>
+        <v>1.009732495170548</v>
       </c>
       <c r="L23">
-        <v>1.00184655625471</v>
+        <v>1.009282063881799</v>
       </c>
       <c r="M23">
-        <v>1.001792585065534</v>
+        <v>1.009229277623229</v>
       </c>
       <c r="N23">
-        <v>1.021479585716867</v>
+        <v>1.021374606082545</v>
       </c>
       <c r="O23">
-        <v>1.019876903148839</v>
+        <v>1.018175334542573</v>
       </c>
       <c r="P23">
-        <v>1.018999126388503</v>
+        <v>1.017296046875873</v>
       </c>
       <c r="Q23">
-        <v>1.002344529711718</v>
+        <v>1.013480744225603</v>
       </c>
       <c r="R23">
-        <v>1.019612208615851</v>
+        <v>1.004566400808182</v>
       </c>
       <c r="S23">
-        <v>1.00259929283158</v>
+        <v>1.001632815461654</v>
       </c>
       <c r="T23">
-        <v>1.001776761182203</v>
+        <v>1.003312372363716</v>
       </c>
       <c r="U23">
-        <v>1.003904912726866</v>
+        <v>1.008104448166963</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1872,61 +1872,61 @@
         <v>1.03</v>
       </c>
       <c r="C24">
-        <v>1.02141591325723</v>
+        <v>1.022083962141479</v>
       </c>
       <c r="D24">
-        <v>1.015641549874597</v>
+        <v>1.019138620706091</v>
       </c>
       <c r="E24">
-        <v>1.006110677680211</v>
+        <v>1.014123165561195</v>
       </c>
       <c r="F24">
-        <v>1.005602421797377</v>
+        <v>1.013594550582936</v>
       </c>
       <c r="G24">
-        <v>1.005250497856304</v>
+        <v>1.013222881345236</v>
       </c>
       <c r="H24">
-        <v>1.004864449035006</v>
+        <v>1.012840714254061</v>
       </c>
       <c r="I24">
-        <v>1.004619785227611</v>
+        <v>1.012263826853184</v>
       </c>
       <c r="J24">
-        <v>1.004664457312333</v>
+        <v>1.012463414222077</v>
       </c>
       <c r="K24">
-        <v>1.004397642763637</v>
+        <v>1.012172283333852</v>
       </c>
       <c r="L24">
-        <v>1.00406066354718</v>
+        <v>1.011774278470051</v>
       </c>
       <c r="M24">
-        <v>1.004007964390359</v>
+        <v>1.011725473789286</v>
       </c>
       <c r="N24">
-        <v>1.022059889098675</v>
+        <v>1.022016073158594</v>
       </c>
       <c r="O24">
-        <v>1.02059753035813</v>
+        <v>1.019688774600598</v>
       </c>
       <c r="P24">
-        <v>1.019776939231271</v>
+        <v>1.018867428860743</v>
       </c>
       <c r="Q24">
-        <v>1.004648588072971</v>
+        <v>1.016441578554025</v>
       </c>
       <c r="R24">
-        <v>1.020457398803088</v>
+        <v>1.009717716317205</v>
       </c>
       <c r="S24">
-        <v>1.004728547089417</v>
+        <v>1.007951890353167</v>
       </c>
       <c r="T24">
-        <v>1.003866039255106</v>
+        <v>1.007460124550489</v>
       </c>
       <c r="U24">
-        <v>1.006094785596281</v>
+        <v>1.014350381352077</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -1937,61 +1937,61 @@
         <v>1.03</v>
       </c>
       <c r="C25">
-        <v>1.021754135059059</v>
+        <v>1.022460844004319</v>
       </c>
       <c r="D25">
-        <v>1.016274825206952</v>
+        <v>1.019833170435913</v>
       </c>
       <c r="E25">
-        <v>1.007200040906886</v>
+        <v>1.015255509173406</v>
       </c>
       <c r="F25">
-        <v>1.006724127681966</v>
+        <v>1.014759530431972</v>
       </c>
       <c r="G25">
-        <v>1.006397889481471</v>
+        <v>1.014413841811292</v>
       </c>
       <c r="H25">
-        <v>1.006025779135655</v>
+        <v>1.014045520400776</v>
       </c>
       <c r="I25">
-        <v>1.005763464679494</v>
+        <v>1.013629827315112</v>
       </c>
       <c r="J25">
-        <v>1.005805167902696</v>
+        <v>1.013769223828401</v>
       </c>
       <c r="K25">
-        <v>1.005547306961417</v>
+        <v>1.013506077489256</v>
       </c>
       <c r="L25">
-        <v>1.005221767299546</v>
+        <v>1.013165289613162</v>
       </c>
       <c r="M25">
-        <v>1.005170869617912</v>
+        <v>1.013118283948881</v>
       </c>
       <c r="N25">
-        <v>1.022319763117604</v>
+        <v>1.022294940271448</v>
       </c>
       <c r="O25">
-        <v>1.020942606382309</v>
+        <v>1.020346897830716</v>
       </c>
       <c r="P25">
-        <v>1.020147695657239</v>
+        <v>1.019551507795671</v>
       </c>
       <c r="Q25">
-        <v>1.005789280637143</v>
+        <v>1.018298202807504</v>
       </c>
       <c r="R25">
-        <v>1.020926480012593</v>
+        <v>1.012095406594763</v>
       </c>
       <c r="S25">
-        <v>1.006256226952764</v>
+        <v>1.010917698587505</v>
       </c>
       <c r="T25">
-        <v>1.005029072429465</v>
+        <v>1.011620259946086</v>
       </c>
       <c r="U25">
-        <v>1.007184131608519</v>
+        <v>1.016999135217193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>